<commit_message>
Update hybrid WENO switch
</commit_message>
<xml_diff>
--- a/doc/WENO2D/stencil.xlsx
+++ b/doc/WENO2D/stencil.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="E:\Study\Models\FVM\doc\WENO2D\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{63A79290-B4F0-4275-A3DF-07872B1D7FE9}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{1D020B52-B7DB-43DA-8A69-103A5695A522}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="4830" yWindow="1386" windowWidth="16650" windowHeight="10206" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-96" yWindow="-96" windowWidth="23232" windowHeight="12552" activeTab="2" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="3rd" sheetId="3" r:id="rId1"/>
@@ -22,7 +22,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="25" uniqueCount="25">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="41" uniqueCount="41">
   <si>
     <t>1</t>
     <phoneticPr fontId="6" type="noConversion"/>
@@ -299,6 +299,147 @@
     </r>
     <phoneticPr fontId="6" type="noConversion"/>
   </si>
+  <si>
+    <t>1</t>
+    <phoneticPr fontId="6" type="noConversion"/>
+  </si>
+  <si>
+    <t>2</t>
+    <phoneticPr fontId="6" type="noConversion"/>
+  </si>
+  <si>
+    <t>3</t>
+    <phoneticPr fontId="6" type="noConversion"/>
+  </si>
+  <si>
+    <t>4</t>
+    <phoneticPr fontId="6" type="noConversion"/>
+  </si>
+  <si>
+    <t>5</t>
+    <phoneticPr fontId="6" type="noConversion"/>
+  </si>
+  <si>
+    <t>6</t>
+    <phoneticPr fontId="6" type="noConversion"/>
+  </si>
+  <si>
+    <t>7</t>
+    <phoneticPr fontId="6" type="noConversion"/>
+  </si>
+  <si>
+    <t>8</t>
+    <phoneticPr fontId="6" type="noConversion"/>
+  </si>
+  <si>
+    <t>9</t>
+    <phoneticPr fontId="6" type="noConversion"/>
+  </si>
+  <si>
+    <r>
+      <t>1</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="12"/>
+        <rFont val="宋体"/>
+        <family val="3"/>
+        <charset val="134"/>
+      </rPr>
+      <t>0</t>
+    </r>
+    <phoneticPr fontId="6" type="noConversion"/>
+  </si>
+  <si>
+    <r>
+      <t>1</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="12"/>
+        <rFont val="宋体"/>
+        <family val="3"/>
+        <charset val="134"/>
+      </rPr>
+      <t>1</t>
+    </r>
+    <phoneticPr fontId="6" type="noConversion"/>
+  </si>
+  <si>
+    <r>
+      <t>1</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="12"/>
+        <rFont val="宋体"/>
+        <family val="3"/>
+        <charset val="134"/>
+      </rPr>
+      <t>2</t>
+    </r>
+    <phoneticPr fontId="6" type="noConversion"/>
+  </si>
+  <si>
+    <r>
+      <t>1</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="12"/>
+        <rFont val="宋体"/>
+        <family val="3"/>
+        <charset val="134"/>
+      </rPr>
+      <t>3</t>
+    </r>
+    <phoneticPr fontId="6" type="noConversion"/>
+  </si>
+  <si>
+    <r>
+      <t>1</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="12"/>
+        <rFont val="宋体"/>
+        <family val="3"/>
+        <charset val="134"/>
+      </rPr>
+      <t>4</t>
+    </r>
+    <phoneticPr fontId="6" type="noConversion"/>
+  </si>
+  <si>
+    <r>
+      <t>1</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="12"/>
+        <rFont val="宋体"/>
+        <family val="3"/>
+        <charset val="134"/>
+      </rPr>
+      <t>5</t>
+    </r>
+    <phoneticPr fontId="6" type="noConversion"/>
+  </si>
+  <si>
+    <r>
+      <t>1</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="12"/>
+        <rFont val="宋体"/>
+        <family val="3"/>
+        <charset val="134"/>
+      </rPr>
+      <t>6</t>
+    </r>
+    <phoneticPr fontId="6" type="noConversion"/>
+  </si>
 </sst>
 </file>
 
@@ -362,7 +503,7 @@
       </patternFill>
     </fill>
   </fills>
-  <borders count="65">
+  <borders count="95">
     <border>
       <left/>
       <right/>
@@ -1165,17 +1306,6 @@
       <diagonal/>
     </border>
     <border>
-      <left style="thin">
-        <color theme="2"/>
-      </left>
-      <right style="thick">
-        <color rgb="FFFF0000"/>
-      </right>
-      <top/>
-      <bottom/>
-      <diagonal/>
-    </border>
-    <border>
       <left style="thick">
         <color rgb="FFFF0000"/>
       </left>
@@ -1190,6 +1320,393 @@
       </bottom>
       <diagonal/>
     </border>
+    <border>
+      <left style="thin">
+        <color theme="2"/>
+      </left>
+      <right/>
+      <top style="thin">
+        <color theme="2"/>
+      </top>
+      <bottom style="thin">
+        <color theme="2"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right style="thick">
+        <color rgb="FFFF0000"/>
+      </right>
+      <top style="thick">
+        <color rgb="FFFF0000"/>
+      </top>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right style="thick">
+        <color rgb="FFFF0000"/>
+      </right>
+      <top/>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right style="thick">
+        <color rgb="FFFF0000"/>
+      </right>
+      <top style="thin">
+        <color indexed="64"/>
+      </top>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right/>
+      <top/>
+      <bottom style="thick">
+        <color rgb="FFFF0000"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right style="thick">
+        <color rgb="FFFF0000"/>
+      </right>
+      <top/>
+      <bottom style="thick">
+        <color rgb="FFFF0000"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thick">
+        <color rgb="FFFF0000"/>
+      </left>
+      <right style="thick">
+        <color rgb="FFFF0000"/>
+      </right>
+      <top/>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right/>
+      <top/>
+      <bottom style="thick">
+        <color rgb="FF00B0F0"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right style="thick">
+        <color rgb="FF00B0F0"/>
+      </right>
+      <top/>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right style="thick">
+        <color rgb="FF00B0F0"/>
+      </right>
+      <top/>
+      <bottom style="thick">
+        <color rgb="FF00B0F0"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thick">
+        <color rgb="FF00B0F0"/>
+      </left>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top style="thick">
+        <color rgb="FF00B0F0"/>
+      </top>
+      <bottom style="thick">
+        <color rgb="FF00B0F0"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right style="thick">
+        <color rgb="FF00B0F0"/>
+      </right>
+      <top style="thick">
+        <color rgb="FF00B0F0"/>
+      </top>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thick">
+        <color rgb="FF00B0F0"/>
+      </left>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top style="thin">
+        <color indexed="64"/>
+      </top>
+      <bottom style="thick">
+        <color rgb="FF00B0F0"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thick">
+        <color rgb="FF00B0F0"/>
+      </left>
+      <right style="thick">
+        <color rgb="FF00B0F0"/>
+      </right>
+      <top style="thin">
+        <color indexed="64"/>
+      </top>
+      <bottom style="thick">
+        <color rgb="FF00B0F0"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right style="thick">
+        <color rgb="FF00B0F0"/>
+      </right>
+      <top style="thin">
+        <color indexed="64"/>
+      </top>
+      <bottom style="thick">
+        <color rgb="FF00B0F0"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right/>
+      <top/>
+      <bottom style="thick">
+        <color rgb="FF00B0F0"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right style="thick">
+        <color rgb="FF00B0F0"/>
+      </right>
+      <top/>
+      <bottom style="thick">
+        <color rgb="FF00B0F0"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right style="thick">
+        <color rgb="FF00B0F0"/>
+      </right>
+      <top/>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thick">
+        <color rgb="FF00B0F0"/>
+      </left>
+      <right style="thick">
+        <color rgb="FF00B0F0"/>
+      </right>
+      <top style="thick">
+        <color rgb="FF00B0F0"/>
+      </top>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thick">
+        <color rgb="FF00B0F0"/>
+      </left>
+      <right style="thick">
+        <color rgb="FF00B0F0"/>
+      </right>
+      <top style="thick">
+        <color rgb="FF00B0F0"/>
+      </top>
+      <bottom style="thick">
+        <color rgb="FF00B0F0"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top style="thick">
+        <color rgb="FFFF0000"/>
+      </top>
+      <bottom style="thick">
+        <color rgb="FFFF0000"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thick">
+        <color rgb="FFFF0000"/>
+      </left>
+      <right/>
+      <top style="thick">
+        <color rgb="FFFF0000"/>
+      </top>
+      <bottom style="thick">
+        <color rgb="FFFF0000"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right style="thick">
+        <color rgb="FFFF0000"/>
+      </right>
+      <top style="thick">
+        <color rgb="FFFF0000"/>
+      </top>
+      <bottom style="thick">
+        <color rgb="FFFF0000"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right/>
+      <top style="thick">
+        <color rgb="FFFF0000"/>
+      </top>
+      <bottom style="thick">
+        <color rgb="FFFF0000"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thick">
+        <color rgb="FFFF0000"/>
+      </left>
+      <right/>
+      <top/>
+      <bottom style="thick">
+        <color rgb="FFFF0000"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thick">
+        <color rgb="FFFF0000"/>
+      </left>
+      <right style="thick">
+        <color rgb="FFFF0000"/>
+      </right>
+      <top/>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right/>
+      <top style="thick">
+        <color rgb="FF00B0F0"/>
+      </top>
+      <bottom style="thick">
+        <color rgb="FF00B0F0"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top style="thick">
+        <color rgb="FF00B0F0"/>
+      </top>
+      <bottom style="thick">
+        <color rgb="FF00B0F0"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thick">
+        <color rgb="FF00B0F0"/>
+      </left>
+      <right style="thick">
+        <color rgb="FF00B0F0"/>
+      </right>
+      <top/>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thick">
+        <color rgb="FF00B0F0"/>
+      </left>
+      <right style="thick">
+        <color rgb="FF00B0F0"/>
+      </right>
+      <top style="thin">
+        <color indexed="64"/>
+      </top>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top/>
+      <bottom style="thick">
+        <color rgb="FF00B0F0"/>
+      </bottom>
+      <diagonal/>
+    </border>
   </borders>
   <cellStyleXfs count="2">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0">
@@ -1199,7 +1716,7 @@
       <alignment vertical="center"/>
     </xf>
   </cellStyleXfs>
-  <cellXfs count="135">
+  <cellXfs count="187">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0">
       <alignment vertical="center"/>
     </xf>
@@ -1599,10 +2116,166 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="62" xfId="0" applyBorder="1">
       <alignment vertical="center"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="63" xfId="0" applyFill="1" applyBorder="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="64" xfId="0" applyFill="1" applyBorder="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="15" xfId="0" applyBorder="1">
+      <alignment vertical="center"/>
+    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="63" xfId="0" applyBorder="1">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="64" xfId="0" applyFill="1" applyBorder="1">
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="65" xfId="0" applyBorder="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="61" xfId="0" applyBorder="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="55" xfId="0" applyBorder="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="66" xfId="0" applyFill="1" applyBorder="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="67" xfId="0" applyBorder="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="26" xfId="0" applyBorder="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="68" xfId="0" applyBorder="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="69" xfId="0" applyBorder="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="54" xfId="0" applyBorder="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="59" xfId="0" applyBorder="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="70" xfId="0" applyBorder="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="71" xfId="0" applyBorder="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="72" xfId="0" applyBorder="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="73" xfId="0" applyBorder="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="74" xfId="0" applyBorder="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="75" xfId="0" applyBorder="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="77" xfId="0" applyBorder="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="79" xfId="0" applyBorder="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="80" xfId="0" applyBorder="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="82" xfId="0" applyBorder="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyBorder="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="83" xfId="0" applyBorder="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="13" xfId="0" applyBorder="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="76" xfId="0" applyFill="1" applyBorder="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="78" xfId="0" applyFill="1" applyBorder="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="81" xfId="0" applyFill="1" applyBorder="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="18" xfId="0" applyBorder="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="33" xfId="0" applyBorder="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="12" xfId="0" applyBorder="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="50" xfId="0" applyBorder="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="25" xfId="0" applyBorder="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="5" xfId="0" applyBorder="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="84" xfId="0" applyBorder="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="85" xfId="0" applyBorder="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="19" xfId="0" applyBorder="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="86" xfId="0" applyBorder="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="87" xfId="0" applyBorder="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="7" xfId="0" applyBorder="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="8" xfId="0" applyBorder="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="88" xfId="0" applyBorder="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="11" xfId="0" applyBorder="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="89" xfId="0" applyBorder="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="90" xfId="0" applyBorder="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="91" xfId="0" applyBorder="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="92" xfId="0" applyBorder="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="93" xfId="0" applyBorder="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="94" xfId="0" applyBorder="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="6" xfId="0" applyBorder="1">
       <alignment vertical="center"/>
     </xf>
   </cellXfs>
@@ -1883,8 +2556,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0200-000000000000}">
   <dimension ref="B1:AI40"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A7" workbookViewId="0">
-      <selection activeCell="N20" sqref="N20"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="U21" sqref="U21"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9" defaultRowHeight="15.3" x14ac:dyDescent="0.45"/>
@@ -1892,10 +2565,10 @@
     <col min="1" max="256" width="2.6484375" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="2:24" ht="16.3" customHeight="1" x14ac:dyDescent="0.45">
+    <row r="1" spans="2:23" ht="16.3" customHeight="1" x14ac:dyDescent="0.45">
       <c r="P1" s="48"/>
     </row>
-    <row r="2" spans="2:24" ht="16.3" customHeight="1" x14ac:dyDescent="0.45">
+    <row r="2" spans="2:23" ht="16.3" customHeight="1" x14ac:dyDescent="0.45">
       <c r="B2" s="52"/>
       <c r="C2" s="50"/>
       <c r="D2" s="50"/>
@@ -1903,14 +2576,14 @@
       <c r="F2" s="50"/>
       <c r="G2" s="50"/>
     </row>
-    <row r="3" spans="2:24" ht="16.3" customHeight="1" x14ac:dyDescent="0.45">
+    <row r="3" spans="2:23" ht="16.3" customHeight="1" x14ac:dyDescent="0.45">
       <c r="C3" s="54"/>
       <c r="D3" s="54"/>
       <c r="E3" s="54"/>
       <c r="F3" s="50"/>
       <c r="G3" s="50"/>
     </row>
-    <row r="4" spans="2:24" ht="16.3" customHeight="1" x14ac:dyDescent="0.45">
+    <row r="4" spans="2:23" ht="16.3" customHeight="1" x14ac:dyDescent="0.45">
       <c r="C4" s="1">
         <v>7</v>
       </c>
@@ -1921,9 +2594,9 @@
         <v>9</v>
       </c>
       <c r="F4" s="53"/>
-      <c r="G4" s="50"/>
-    </row>
-    <row r="5" spans="2:24" ht="16.3" customHeight="1" x14ac:dyDescent="0.45">
+      <c r="G4" s="134"/>
+    </row>
+    <row r="5" spans="2:23" ht="16.3" customHeight="1" x14ac:dyDescent="0.45">
       <c r="C5" s="1">
         <v>4</v>
       </c>
@@ -1936,7 +2609,7 @@
       <c r="F5" s="53"/>
       <c r="G5" s="50"/>
     </row>
-    <row r="6" spans="2:24" ht="16.3" customHeight="1" x14ac:dyDescent="0.45">
+    <row r="6" spans="2:23" ht="16.3" customHeight="1" x14ac:dyDescent="0.45">
       <c r="C6" s="1">
         <v>1</v>
       </c>
@@ -1949,10 +2622,10 @@
       <c r="F6" s="53"/>
       <c r="G6" s="50"/>
     </row>
-    <row r="7" spans="2:24" x14ac:dyDescent="0.45">
+    <row r="7" spans="2:23" x14ac:dyDescent="0.45">
       <c r="R7" s="49"/>
     </row>
-    <row r="8" spans="2:24" ht="16.3" customHeight="1" thickBot="1" x14ac:dyDescent="0.5">
+    <row r="8" spans="2:23" ht="16.3" customHeight="1" thickBot="1" x14ac:dyDescent="0.5">
       <c r="C8" s="55">
         <v>1</v>
       </c>
@@ -1977,11 +2650,11 @@
       <c r="R8" s="56"/>
       <c r="S8" s="56"/>
       <c r="T8" s="56"/>
-      <c r="V8" s="61">
+      <c r="U8" s="61">
         <v>4</v>
       </c>
     </row>
-    <row r="9" spans="2:24" ht="16.3" customHeight="1" thickTop="1" thickBot="1" x14ac:dyDescent="0.5">
+    <row r="9" spans="2:23" ht="16.3" customHeight="1" thickTop="1" thickBot="1" x14ac:dyDescent="0.5">
       <c r="C9" s="18">
         <v>7</v>
       </c>
@@ -2018,17 +2691,17 @@
       <c r="R9" s="53"/>
       <c r="S9" s="50"/>
       <c r="T9" s="56"/>
-      <c r="V9" s="12">
+      <c r="U9" s="12">
         <v>7</v>
       </c>
-      <c r="W9" s="9">
+      <c r="V9" s="9">
         <v>8</v>
       </c>
-      <c r="X9" s="5">
+      <c r="W9" s="5">
         <v>9</v>
       </c>
     </row>
-    <row r="10" spans="2:24" ht="16.3" customHeight="1" thickTop="1" thickBot="1" x14ac:dyDescent="0.5">
+    <row r="10" spans="2:23" ht="16.3" customHeight="1" thickTop="1" thickBot="1" x14ac:dyDescent="0.5">
       <c r="C10" s="9">
         <v>4</v>
       </c>
@@ -2065,17 +2738,17 @@
       <c r="R10" s="53"/>
       <c r="S10" s="50"/>
       <c r="T10" s="56"/>
-      <c r="V10" s="12">
+      <c r="U10" s="12">
         <v>4</v>
       </c>
-      <c r="W10" s="11">
+      <c r="V10" s="11">
         <v>5</v>
       </c>
-      <c r="X10" s="8">
+      <c r="W10" s="8">
         <v>6</v>
       </c>
     </row>
-    <row r="11" spans="2:24" ht="16.3" customHeight="1" thickTop="1" thickBot="1" x14ac:dyDescent="0.5">
+    <row r="11" spans="2:23" ht="16.3" customHeight="1" thickTop="1" thickBot="1" x14ac:dyDescent="0.5">
       <c r="C11" s="11">
         <v>1</v>
       </c>
@@ -2112,17 +2785,17 @@
       <c r="R11" s="50"/>
       <c r="S11" s="50"/>
       <c r="T11" s="56"/>
-      <c r="V11" s="1">
+      <c r="U11" s="1">
         <v>1</v>
       </c>
+      <c r="V11" s="3">
+        <v>2</v>
+      </c>
       <c r="W11" s="3">
-        <v>2</v>
-      </c>
-      <c r="X11" s="3">
         <v>3</v>
       </c>
     </row>
-    <row r="12" spans="2:24" ht="16.3" customHeight="1" thickTop="1" x14ac:dyDescent="0.45">
+    <row r="12" spans="2:23" ht="16.3" customHeight="1" thickTop="1" x14ac:dyDescent="0.45">
       <c r="C12" s="51"/>
       <c r="D12" s="51"/>
       <c r="E12" s="50"/>
@@ -2142,7 +2815,7 @@
       <c r="S12" s="50"/>
       <c r="T12" s="56"/>
     </row>
-    <row r="13" spans="2:24" ht="16.3" customHeight="1" thickBot="1" x14ac:dyDescent="0.5">
+    <row r="13" spans="2:23" ht="16.3" customHeight="1" thickBot="1" x14ac:dyDescent="0.5">
       <c r="C13" s="124">
         <v>1</v>
       </c>
@@ -2167,13 +2840,13 @@
       <c r="R13" s="56"/>
       <c r="S13" s="56"/>
       <c r="T13" s="56"/>
-      <c r="V13" s="131">
+      <c r="U13" s="131">
         <v>4</v>
       </c>
+      <c r="V13" s="132"/>
       <c r="W13" s="132"/>
-      <c r="X13" s="132"/>
-    </row>
-    <row r="14" spans="2:24" ht="16.3" customHeight="1" thickTop="1" thickBot="1" x14ac:dyDescent="0.5">
+    </row>
+    <row r="14" spans="2:23" ht="16.3" customHeight="1" thickTop="1" thickBot="1" x14ac:dyDescent="0.5">
       <c r="B14" s="123"/>
       <c r="C14" s="121">
         <v>7</v>
@@ -2211,18 +2884,17 @@
       <c r="R14" s="126"/>
       <c r="S14" s="56"/>
       <c r="T14" s="56"/>
-      <c r="U14" s="133"/>
-      <c r="V14" s="134">
+      <c r="U14" s="133">
         <v>7</v>
       </c>
-      <c r="W14" s="3">
+      <c r="V14" s="3">
         <v>8</v>
       </c>
-      <c r="X14" s="5">
+      <c r="W14" s="5">
         <v>9</v>
       </c>
     </row>
-    <row r="15" spans="2:24" ht="16.3" customHeight="1" thickTop="1" thickBot="1" x14ac:dyDescent="0.5">
+    <row r="15" spans="2:23" ht="16.3" customHeight="1" thickTop="1" thickBot="1" x14ac:dyDescent="0.5">
       <c r="B15" s="123"/>
       <c r="C15" s="2">
         <v>4</v>
@@ -2260,17 +2932,17 @@
       <c r="R15" s="50"/>
       <c r="S15" s="50"/>
       <c r="T15" s="56"/>
-      <c r="V15" s="5">
+      <c r="U15" s="5">
         <v>4</v>
       </c>
-      <c r="W15" s="11">
+      <c r="V15" s="11">
         <v>5</v>
       </c>
-      <c r="X15" s="6">
+      <c r="W15" s="6">
         <v>6</v>
       </c>
     </row>
-    <row r="16" spans="2:24" ht="16.3" customHeight="1" thickTop="1" thickBot="1" x14ac:dyDescent="0.5">
+    <row r="16" spans="2:23" ht="16.3" customHeight="1" thickTop="1" thickBot="1" x14ac:dyDescent="0.5">
       <c r="B16" s="123"/>
       <c r="C16" s="11">
         <v>1</v>
@@ -2307,13 +2979,13 @@
       </c>
       <c r="S16" s="50"/>
       <c r="T16" s="56"/>
-      <c r="V16" s="1">
+      <c r="U16" s="1">
         <v>1</v>
       </c>
-      <c r="W16" s="5">
+      <c r="V16" s="5">
         <v>2</v>
       </c>
-      <c r="X16" s="122">
+      <c r="W16" s="122">
         <v>3</v>
       </c>
     </row>
@@ -3020,10 +3692,10 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
-  <dimension ref="C1:AE38"/>
+  <dimension ref="C1:CY38"/>
   <sheetViews>
     <sheetView zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="X13" sqref="X13"/>
+      <selection activeCell="BV19" sqref="BV19"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9" defaultRowHeight="16.3" customHeight="1" x14ac:dyDescent="0.45"/>
@@ -3031,10 +3703,12 @@
     <col min="1" max="256" width="2.6484375" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="3:29" ht="16.3" customHeight="1" thickBot="1" x14ac:dyDescent="0.5">
+    <row r="1" spans="3:103" ht="16.3" customHeight="1" thickBot="1" x14ac:dyDescent="0.5">
       <c r="P1" s="48"/>
-    </row>
-    <row r="2" spans="3:29" ht="16.3" customHeight="1" thickTop="1" thickBot="1" x14ac:dyDescent="0.5">
+      <c r="AU1" s="149"/>
+      <c r="CD1" s="149"/>
+    </row>
+    <row r="2" spans="3:103" ht="16.3" customHeight="1" thickTop="1" thickBot="1" x14ac:dyDescent="0.5">
       <c r="C2" s="19">
         <v>21</v>
       </c>
@@ -3055,8 +3729,13 @@
       <c r="Z2" s="114"/>
       <c r="AA2" s="114"/>
       <c r="AB2" s="115"/>
-    </row>
-    <row r="3" spans="3:29" ht="16.3" customHeight="1" thickTop="1" x14ac:dyDescent="0.45">
+      <c r="AT2" s="151"/>
+      <c r="AU2" s="159"/>
+      <c r="AV2" s="149"/>
+      <c r="CC2" s="150"/>
+      <c r="CD2" s="157"/>
+    </row>
+    <row r="3" spans="3:103" ht="16.3" customHeight="1" thickTop="1" thickBot="1" x14ac:dyDescent="0.5">
       <c r="C3" s="12">
         <v>16</v>
       </c>
@@ -3089,8 +3768,25 @@
         <v>25</v>
       </c>
       <c r="AC3" s="118"/>
-    </row>
-    <row r="4" spans="3:29" ht="16.3" customHeight="1" x14ac:dyDescent="0.45">
+      <c r="AI3" s="135">
+        <v>13</v>
+      </c>
+      <c r="AS3" s="151"/>
+      <c r="AT3" s="159"/>
+      <c r="AU3" s="157">
+        <v>13</v>
+      </c>
+      <c r="AV3" s="115"/>
+      <c r="AW3" s="149"/>
+      <c r="BQ3" s="165">
+        <v>9</v>
+      </c>
+      <c r="CC3" s="150"/>
+      <c r="CD3" s="184">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="4" spans="3:103" ht="16.3" customHeight="1" thickTop="1" thickBot="1" x14ac:dyDescent="0.5">
       <c r="C4" s="12">
         <v>11</v>
       </c>
@@ -3123,8 +3819,43 @@
         <v>20</v>
       </c>
       <c r="AC4" s="119"/>
-    </row>
-    <row r="5" spans="3:29" ht="16.3" customHeight="1" x14ac:dyDescent="0.45">
+      <c r="AH4" s="1">
+        <v>10</v>
+      </c>
+      <c r="AI4" s="1">
+        <v>11</v>
+      </c>
+      <c r="AJ4" s="1">
+        <v>12</v>
+      </c>
+      <c r="AK4" s="136"/>
+      <c r="AR4" s="151"/>
+      <c r="AS4" s="159"/>
+      <c r="AT4" s="13">
+        <v>10</v>
+      </c>
+      <c r="AU4" s="1">
+        <v>11</v>
+      </c>
+      <c r="AV4" s="164">
+        <v>12</v>
+      </c>
+      <c r="AW4" s="115"/>
+      <c r="AX4" s="149"/>
+      <c r="BQ4" s="166">
+        <v>8</v>
+      </c>
+      <c r="CA4" s="149"/>
+      <c r="CB4" s="149"/>
+      <c r="CC4" s="151"/>
+      <c r="CD4" s="183">
+        <v>8</v>
+      </c>
+      <c r="CE4" s="149"/>
+      <c r="CF4" s="149"/>
+      <c r="CG4" s="149"/>
+    </row>
+    <row r="5" spans="3:103" ht="16.3" customHeight="1" thickTop="1" thickBot="1" x14ac:dyDescent="0.5">
       <c r="C5" s="12">
         <v>6</v>
       </c>
@@ -3157,8 +3888,74 @@
         <v>15</v>
       </c>
       <c r="AC5" s="119"/>
-    </row>
-    <row r="6" spans="3:29" ht="16.3" customHeight="1" x14ac:dyDescent="0.45">
+      <c r="AG5" s="135">
+        <v>5</v>
+      </c>
+      <c r="AH5" s="1">
+        <v>6</v>
+      </c>
+      <c r="AI5" s="1">
+        <v>7</v>
+      </c>
+      <c r="AJ5" s="1">
+        <v>8</v>
+      </c>
+      <c r="AK5" s="135">
+        <v>9</v>
+      </c>
+      <c r="AQ5" s="150"/>
+      <c r="AR5" s="159"/>
+      <c r="AS5" s="152">
+        <v>5</v>
+      </c>
+      <c r="AT5" s="1">
+        <v>6</v>
+      </c>
+      <c r="AU5" s="1">
+        <v>7</v>
+      </c>
+      <c r="AV5" s="1">
+        <v>8</v>
+      </c>
+      <c r="AW5" s="156">
+        <v>9</v>
+      </c>
+      <c r="AX5" s="151"/>
+      <c r="BO5" s="167">
+        <v>3</v>
+      </c>
+      <c r="BP5" s="168">
+        <v>4</v>
+      </c>
+      <c r="BQ5" s="135">
+        <v>5</v>
+      </c>
+      <c r="BR5" s="168">
+        <v>6</v>
+      </c>
+      <c r="BS5" s="162">
+        <v>7</v>
+      </c>
+      <c r="BZ5" s="150"/>
+      <c r="CA5" s="152"/>
+      <c r="CB5" s="181">
+        <v>3</v>
+      </c>
+      <c r="CC5" s="182">
+        <v>4</v>
+      </c>
+      <c r="CD5" s="135">
+        <v>5</v>
+      </c>
+      <c r="CE5" s="155">
+        <v>6</v>
+      </c>
+      <c r="CF5" s="185">
+        <v>7</v>
+      </c>
+      <c r="CG5" s="156"/>
+    </row>
+    <row r="6" spans="3:103" ht="16.3" customHeight="1" thickTop="1" thickBot="1" x14ac:dyDescent="0.5">
       <c r="C6" s="1">
         <v>1</v>
       </c>
@@ -3191,8 +3988,36 @@
         <v>10</v>
       </c>
       <c r="AC6" s="119"/>
-    </row>
-    <row r="7" spans="3:29" ht="16.3" customHeight="1" thickBot="1" x14ac:dyDescent="0.5">
+      <c r="AH6" s="1">
+        <v>2</v>
+      </c>
+      <c r="AI6" s="1">
+        <v>3</v>
+      </c>
+      <c r="AJ6" s="1">
+        <v>4</v>
+      </c>
+      <c r="AR6" s="153"/>
+      <c r="AS6" s="159"/>
+      <c r="AT6" s="161">
+        <v>2</v>
+      </c>
+      <c r="AU6" s="1">
+        <v>3</v>
+      </c>
+      <c r="AV6" s="163">
+        <v>4</v>
+      </c>
+      <c r="AW6" s="151"/>
+      <c r="BQ6" s="166">
+        <v>2</v>
+      </c>
+      <c r="CC6" s="153"/>
+      <c r="CD6" s="184">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="7" spans="3:103" ht="16.3" customHeight="1" thickTop="1" thickBot="1" x14ac:dyDescent="0.5">
       <c r="W7" s="120"/>
       <c r="X7" s="16">
         <v>1</v>
@@ -3210,8 +4035,24 @@
         <v>5</v>
       </c>
       <c r="AC7" s="120"/>
-    </row>
-    <row r="8" spans="3:29" ht="16.3" customHeight="1" thickTop="1" thickBot="1" x14ac:dyDescent="0.5">
+      <c r="AI7" s="135">
+        <v>1</v>
+      </c>
+      <c r="AS7" s="153"/>
+      <c r="AT7" s="159"/>
+      <c r="AU7" s="154">
+        <v>1</v>
+      </c>
+      <c r="AV7" s="151"/>
+      <c r="BQ7" s="158">
+        <v>1</v>
+      </c>
+      <c r="CC7" s="150"/>
+      <c r="CD7" s="183">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="8" spans="3:103" ht="16.3" customHeight="1" thickTop="1" thickBot="1" x14ac:dyDescent="0.5">
       <c r="C8" s="38">
         <v>1</v>
       </c>
@@ -3226,8 +4067,12 @@
       <c r="Z8" s="114"/>
       <c r="AA8" s="114"/>
       <c r="AB8" s="115"/>
-    </row>
-    <row r="9" spans="3:29" ht="16.3" customHeight="1" thickTop="1" x14ac:dyDescent="0.45">
+      <c r="AT8" s="153"/>
+      <c r="AU8" s="120"/>
+      <c r="CC8" s="150"/>
+      <c r="CD8" s="154"/>
+    </row>
+    <row r="9" spans="3:103" ht="16.3" customHeight="1" thickTop="1" thickBot="1" x14ac:dyDescent="0.5">
       <c r="C9" s="19">
         <v>21</v>
       </c>
@@ -3273,8 +4118,12 @@
       <c r="S9" s="1">
         <v>25</v>
       </c>
-    </row>
-    <row r="10" spans="3:29" ht="16.3" customHeight="1" thickBot="1" x14ac:dyDescent="0.5">
+      <c r="AY9" s="132"/>
+      <c r="BG9" s="132"/>
+      <c r="CO9" s="132"/>
+      <c r="CW9" s="132"/>
+    </row>
+    <row r="10" spans="3:103" ht="16.3" customHeight="1" thickTop="1" thickBot="1" x14ac:dyDescent="0.5">
       <c r="C10" s="14">
         <v>16</v>
       </c>
@@ -3320,8 +4169,40 @@
       <c r="S10" s="16">
         <v>20</v>
       </c>
-    </row>
-    <row r="11" spans="3:29" ht="16.3" customHeight="1" thickTop="1" x14ac:dyDescent="0.45">
+      <c r="AI10" s="135">
+        <v>13</v>
+      </c>
+      <c r="AQ10" s="135">
+        <v>13</v>
+      </c>
+      <c r="AX10" s="145"/>
+      <c r="AY10" s="146">
+        <v>13</v>
+      </c>
+      <c r="BF10" s="147"/>
+      <c r="BG10" s="148">
+        <v>13</v>
+      </c>
+      <c r="BH10" s="132"/>
+      <c r="BQ10" s="176">
+        <v>9</v>
+      </c>
+      <c r="BY10" s="165">
+        <v>9</v>
+      </c>
+      <c r="CG10" s="165">
+        <v>9</v>
+      </c>
+      <c r="CN10" s="123"/>
+      <c r="CO10" s="123">
+        <v>9</v>
+      </c>
+      <c r="CV10" s="123"/>
+      <c r="CW10" s="180">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="11" spans="3:103" ht="16.3" customHeight="1" thickTop="1" thickBot="1" x14ac:dyDescent="0.5">
       <c r="C11" s="17">
         <v>11</v>
       </c>
@@ -3367,8 +4248,76 @@
       <c r="S11" s="31">
         <v>15</v>
       </c>
-    </row>
-    <row r="12" spans="3:29" ht="16.3" customHeight="1" x14ac:dyDescent="0.45">
+      <c r="AG11" s="139"/>
+      <c r="AH11" s="7">
+        <v>10</v>
+      </c>
+      <c r="AI11" s="7">
+        <v>11</v>
+      </c>
+      <c r="AJ11" s="1">
+        <v>12</v>
+      </c>
+      <c r="AK11" s="136"/>
+      <c r="AP11" s="1">
+        <v>10</v>
+      </c>
+      <c r="AQ11" s="7">
+        <v>11</v>
+      </c>
+      <c r="AR11" s="7">
+        <v>12</v>
+      </c>
+      <c r="AS11" s="144"/>
+      <c r="AW11" s="145"/>
+      <c r="AX11" s="13">
+        <v>10</v>
+      </c>
+      <c r="AY11" s="6">
+        <v>11</v>
+      </c>
+      <c r="AZ11" s="2">
+        <v>12</v>
+      </c>
+      <c r="BA11" s="136"/>
+      <c r="BF11" s="6">
+        <v>10</v>
+      </c>
+      <c r="BG11" s="2">
+        <v>11</v>
+      </c>
+      <c r="BH11" s="141">
+        <v>12</v>
+      </c>
+      <c r="BI11" s="132"/>
+      <c r="BP11" s="145"/>
+      <c r="BQ11" s="146">
+        <v>8</v>
+      </c>
+      <c r="BR11" s="132"/>
+      <c r="BW11" s="132"/>
+      <c r="BX11" s="139"/>
+      <c r="BY11" s="169">
+        <v>8</v>
+      </c>
+      <c r="CG11" s="169">
+        <v>8</v>
+      </c>
+      <c r="CH11" s="144"/>
+      <c r="CI11" s="132"/>
+      <c r="CM11" s="132"/>
+      <c r="CN11" s="145"/>
+      <c r="CO11" s="147">
+        <v>8</v>
+      </c>
+      <c r="CV11" s="147"/>
+      <c r="CW11" s="148">
+        <v>8</v>
+      </c>
+      <c r="CX11" s="132"/>
+      <c r="CY11" s="132"/>
+    </row>
+    <row r="12" spans="3:103" ht="16.3" customHeight="1" thickTop="1" thickBot="1" x14ac:dyDescent="0.5">
       <c r="C12" s="27">
         <v>6</v>
       </c>
@@ -3414,8 +4363,147 @@
       <c r="S12" s="20">
         <v>10</v>
       </c>
-    </row>
-    <row r="13" spans="3:29" ht="16.3" customHeight="1" thickBot="1" x14ac:dyDescent="0.5">
+      <c r="AF12" s="123"/>
+      <c r="AG12" s="137">
+        <v>5</v>
+      </c>
+      <c r="AH12" s="3">
+        <v>6</v>
+      </c>
+      <c r="AI12" s="141">
+        <v>7</v>
+      </c>
+      <c r="AJ12" s="2">
+        <v>8</v>
+      </c>
+      <c r="AK12" s="135">
+        <v>9</v>
+      </c>
+      <c r="AO12" s="135">
+        <v>5</v>
+      </c>
+      <c r="AP12" s="6">
+        <v>6</v>
+      </c>
+      <c r="AQ12" s="13">
+        <v>7</v>
+      </c>
+      <c r="AR12" s="3">
+        <v>8</v>
+      </c>
+      <c r="AS12" s="143">
+        <v>9</v>
+      </c>
+      <c r="AV12" s="123"/>
+      <c r="AW12" s="139">
+        <v>5</v>
+      </c>
+      <c r="AX12" s="7">
+        <v>6</v>
+      </c>
+      <c r="AY12" s="8">
+        <v>7</v>
+      </c>
+      <c r="AZ12" s="2">
+        <v>8</v>
+      </c>
+      <c r="BA12" s="135">
+        <v>9</v>
+      </c>
+      <c r="BE12" s="135">
+        <v>5</v>
+      </c>
+      <c r="BF12" s="6">
+        <v>6</v>
+      </c>
+      <c r="BG12" s="11">
+        <v>7</v>
+      </c>
+      <c r="BH12" s="7">
+        <v>8</v>
+      </c>
+      <c r="BI12" s="143">
+        <v>9</v>
+      </c>
+      <c r="BO12" s="186">
+        <v>3</v>
+      </c>
+      <c r="BP12" s="137">
+        <v>4</v>
+      </c>
+      <c r="BQ12" s="135">
+        <v>5</v>
+      </c>
+      <c r="BR12" s="143">
+        <v>6</v>
+      </c>
+      <c r="BS12" s="162">
+        <v>7</v>
+      </c>
+      <c r="BV12" s="123"/>
+      <c r="BW12" s="172">
+        <v>3</v>
+      </c>
+      <c r="BX12" s="171">
+        <v>4</v>
+      </c>
+      <c r="BY12" s="170">
+        <v>5</v>
+      </c>
+      <c r="BZ12" s="168">
+        <v>6</v>
+      </c>
+      <c r="CA12" s="162">
+        <v>7</v>
+      </c>
+      <c r="CE12" s="167">
+        <v>3</v>
+      </c>
+      <c r="CF12" s="173">
+        <v>4</v>
+      </c>
+      <c r="CG12" s="160">
+        <v>5</v>
+      </c>
+      <c r="CH12" s="175">
+        <v>6</v>
+      </c>
+      <c r="CI12" s="174">
+        <v>7</v>
+      </c>
+      <c r="CL12" s="123"/>
+      <c r="CM12" s="178">
+        <v>3</v>
+      </c>
+      <c r="CN12" s="139">
+        <v>4</v>
+      </c>
+      <c r="CO12" s="177">
+        <v>5</v>
+      </c>
+      <c r="CP12" s="168">
+        <v>6</v>
+      </c>
+      <c r="CQ12" s="162">
+        <v>7</v>
+      </c>
+      <c r="CU12" s="167">
+        <v>3</v>
+      </c>
+      <c r="CV12" s="173">
+        <v>4</v>
+      </c>
+      <c r="CW12" s="179">
+        <v>5</v>
+      </c>
+      <c r="CX12" s="144">
+        <v>6</v>
+      </c>
+      <c r="CY12" s="145">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="13" spans="3:103" ht="16.3" customHeight="1" thickTop="1" thickBot="1" x14ac:dyDescent="0.5">
       <c r="C13" s="11">
         <v>1</v>
       </c>
@@ -3461,8 +4549,63 @@
       <c r="S13" s="8">
         <v>5</v>
       </c>
-    </row>
-    <row r="14" spans="3:29" ht="16.3" customHeight="1" thickTop="1" x14ac:dyDescent="0.45">
+      <c r="AG13" s="138"/>
+      <c r="AH13" s="11">
+        <v>2</v>
+      </c>
+      <c r="AI13" s="6">
+        <v>3</v>
+      </c>
+      <c r="AJ13" s="2">
+        <v>4</v>
+      </c>
+      <c r="AP13" s="6">
+        <v>2</v>
+      </c>
+      <c r="AQ13" s="2">
+        <v>3</v>
+      </c>
+      <c r="AR13" s="8">
+        <v>4</v>
+      </c>
+      <c r="AX13" s="3">
+        <v>2</v>
+      </c>
+      <c r="AY13" s="3">
+        <v>3</v>
+      </c>
+      <c r="AZ13" s="1">
+        <v>4</v>
+      </c>
+      <c r="BF13" s="1">
+        <v>2</v>
+      </c>
+      <c r="BG13" s="3">
+        <v>3</v>
+      </c>
+      <c r="BH13" s="3">
+        <v>4</v>
+      </c>
+      <c r="BP13" s="138"/>
+      <c r="BQ13" s="140">
+        <v>2</v>
+      </c>
+      <c r="BX13" s="123"/>
+      <c r="BY13" s="142">
+        <v>2</v>
+      </c>
+      <c r="CF13" s="142"/>
+      <c r="CG13" s="142">
+        <v>2</v>
+      </c>
+      <c r="CO13" s="166">
+        <v>2</v>
+      </c>
+      <c r="CW13" s="166">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="14" spans="3:103" ht="16.3" customHeight="1" thickTop="1" thickBot="1" x14ac:dyDescent="0.5">
       <c r="C14" s="40">
         <v>4</v>
       </c>
@@ -3472,8 +4615,39 @@
       <c r="O14" s="42">
         <v>6</v>
       </c>
-    </row>
-    <row r="15" spans="3:29" ht="16.3" customHeight="1" thickBot="1" x14ac:dyDescent="0.5">
+      <c r="AH14" s="138"/>
+      <c r="AI14" s="140">
+        <v>1</v>
+      </c>
+      <c r="AP14" s="142"/>
+      <c r="AQ14" s="140">
+        <v>1</v>
+      </c>
+      <c r="AY14" s="135">
+        <v>1</v>
+      </c>
+      <c r="BG14" s="135">
+        <v>1</v>
+      </c>
+      <c r="BQ14" s="158">
+        <v>1</v>
+      </c>
+      <c r="BX14" s="123"/>
+      <c r="BY14" s="145">
+        <v>1</v>
+      </c>
+      <c r="CF14" s="123"/>
+      <c r="CG14" s="145">
+        <v>1</v>
+      </c>
+      <c r="CO14" s="158">
+        <v>1</v>
+      </c>
+      <c r="CW14" s="158">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="15" spans="3:103" ht="16.3" customHeight="1" thickTop="1" thickBot="1" x14ac:dyDescent="0.5">
       <c r="C15" s="21">
         <v>21</v>
       </c>
@@ -3520,7 +4694,7 @@
         <v>25</v>
       </c>
     </row>
-    <row r="16" spans="3:29" ht="16.3" customHeight="1" thickTop="1" thickBot="1" x14ac:dyDescent="0.5">
+    <row r="16" spans="3:103" ht="16.3" customHeight="1" thickTop="1" thickBot="1" x14ac:dyDescent="0.5">
       <c r="C16" s="23">
         <v>16</v>
       </c>
@@ -3567,7 +4741,7 @@
         <v>20</v>
       </c>
     </row>
-    <row r="17" spans="3:31" ht="16.3" customHeight="1" x14ac:dyDescent="0.45">
+    <row r="17" spans="3:37" ht="16.3" customHeight="1" x14ac:dyDescent="0.45">
       <c r="C17" s="25">
         <v>11</v>
       </c>
@@ -3613,8 +4787,11 @@
       <c r="S17" s="20">
         <v>15</v>
       </c>
-    </row>
-    <row r="18" spans="3:31" ht="16.3" customHeight="1" thickBot="1" x14ac:dyDescent="0.5">
+      <c r="AI17" s="135">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="18" spans="3:37" ht="16.3" customHeight="1" thickBot="1" x14ac:dyDescent="0.5">
       <c r="C18" s="26">
         <v>6</v>
       </c>
@@ -3660,8 +4837,16 @@
       <c r="S18" s="32">
         <v>10</v>
       </c>
-    </row>
-    <row r="19" spans="3:31" ht="16.3" customHeight="1" thickTop="1" x14ac:dyDescent="0.45">
+      <c r="AH18" s="1">
+        <v>10</v>
+      </c>
+      <c r="AI18" s="1">
+        <v>11</v>
+      </c>
+      <c r="AJ18" s="1"/>
+      <c r="AK18" s="136"/>
+    </row>
+    <row r="19" spans="3:37" ht="16.3" customHeight="1" thickTop="1" x14ac:dyDescent="0.45">
       <c r="C19" s="3">
         <v>1</v>
       </c>
@@ -3707,8 +4892,23 @@
       <c r="S19" s="3">
         <v>5</v>
       </c>
-    </row>
-    <row r="20" spans="3:31" ht="16.3" customHeight="1" thickBot="1" x14ac:dyDescent="0.5">
+      <c r="AG19" s="135">
+        <v>5</v>
+      </c>
+      <c r="AH19" s="1">
+        <v>6</v>
+      </c>
+      <c r="AI19" s="1">
+        <v>7</v>
+      </c>
+      <c r="AJ19" s="1">
+        <v>8</v>
+      </c>
+      <c r="AK19" s="135">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="20" spans="3:37" ht="16.3" customHeight="1" thickBot="1" x14ac:dyDescent="0.5">
       <c r="C20" s="41">
         <v>7</v>
       </c>
@@ -3718,8 +4918,17 @@
       <c r="O20" s="38">
         <v>9</v>
       </c>
-    </row>
-    <row r="21" spans="3:31" ht="16.3" customHeight="1" thickTop="1" x14ac:dyDescent="0.45">
+      <c r="AH20" s="1">
+        <v>2</v>
+      </c>
+      <c r="AI20" s="1">
+        <v>3</v>
+      </c>
+      <c r="AJ20" s="1">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="21" spans="3:37" ht="16.3" customHeight="1" thickTop="1" x14ac:dyDescent="0.45">
       <c r="C21" s="36">
         <v>21</v>
       </c>
@@ -3765,8 +4974,11 @@
       <c r="S21" s="5">
         <v>25</v>
       </c>
-    </row>
-    <row r="22" spans="3:31" ht="16.3" customHeight="1" x14ac:dyDescent="0.45">
+      <c r="AI21" s="135">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="22" spans="3:37" ht="16.3" customHeight="1" x14ac:dyDescent="0.45">
       <c r="C22" s="27">
         <v>16</v>
       </c>
@@ -3813,7 +5025,7 @@
         <v>20</v>
       </c>
     </row>
-    <row r="23" spans="3:31" ht="16.3" customHeight="1" thickBot="1" x14ac:dyDescent="0.5">
+    <row r="23" spans="3:37" ht="16.3" customHeight="1" thickBot="1" x14ac:dyDescent="0.5">
       <c r="C23" s="26">
         <v>11</v>
       </c>
@@ -3860,7 +5072,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="24" spans="3:31" ht="16.3" customHeight="1" thickTop="1" x14ac:dyDescent="0.45">
+    <row r="24" spans="3:37" ht="16.3" customHeight="1" thickTop="1" x14ac:dyDescent="0.45">
       <c r="C24" s="15">
         <v>6</v>
       </c>
@@ -3907,7 +5119,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="25" spans="3:31" ht="16.3" customHeight="1" x14ac:dyDescent="0.45">
+    <row r="25" spans="3:37" ht="16.3" customHeight="1" x14ac:dyDescent="0.45">
       <c r="C25" s="1">
         <v>1</v>
       </c>
@@ -3954,7 +5166,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="27" spans="3:31" ht="16.3" customHeight="1" x14ac:dyDescent="0.45">
+    <row r="27" spans="3:37" ht="16.3" customHeight="1" x14ac:dyDescent="0.45">
       <c r="C27" s="37">
         <v>1</v>
       </c>
@@ -3971,7 +5183,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="28" spans="3:31" ht="16.3" customHeight="1" x14ac:dyDescent="0.45">
+    <row r="28" spans="3:37" ht="16.3" customHeight="1" x14ac:dyDescent="0.45">
       <c r="C28" s="19">
         <v>21</v>
       </c>
@@ -4036,7 +5248,7 @@
       </c>
       <c r="AE28" s="1"/>
     </row>
-    <row r="29" spans="3:31" ht="16.3" customHeight="1" x14ac:dyDescent="0.45">
+    <row r="29" spans="3:37" ht="16.3" customHeight="1" x14ac:dyDescent="0.45">
       <c r="C29" s="12">
         <v>16</v>
       </c>
@@ -4107,7 +5319,7 @@
         <v>20</v>
       </c>
     </row>
-    <row r="30" spans="3:31" ht="16.3" customHeight="1" x14ac:dyDescent="0.45">
+    <row r="30" spans="3:37" ht="16.3" customHeight="1" x14ac:dyDescent="0.45">
       <c r="C30" s="12">
         <v>11</v>
       </c>
@@ -4184,7 +5396,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="31" spans="3:31" ht="16.3" customHeight="1" x14ac:dyDescent="0.45">
+    <row r="31" spans="3:37" ht="16.3" customHeight="1" x14ac:dyDescent="0.45">
       <c r="C31" s="12">
         <v>6</v>
       </c>
@@ -4261,7 +5473,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="32" spans="3:31" ht="16.3" customHeight="1" x14ac:dyDescent="0.45">
+    <row r="32" spans="3:37" ht="16.3" customHeight="1" x14ac:dyDescent="0.45">
       <c r="C32" s="1">
         <v>1</v>
       </c>
@@ -4658,10 +5870,10 @@
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{4DC72680-F9AF-4568-9FB8-39F80A980EEB}">
-  <dimension ref="B1:AT83"/>
+  <dimension ref="B1:CJ83"/>
   <sheetViews>
-    <sheetView topLeftCell="A58" workbookViewId="0">
-      <selection activeCell="AG75" sqref="AG75"/>
+    <sheetView tabSelected="1" topLeftCell="W31" workbookViewId="0">
+      <selection activeCell="BT47" sqref="BT47"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9" defaultRowHeight="15.3" x14ac:dyDescent="0.45"/>
@@ -4670,7 +5882,7 @@
     <col min="257" max="16384" width="9" style="62"/>
   </cols>
   <sheetData>
-    <row r="1" spans="2:45" ht="16.3" customHeight="1" x14ac:dyDescent="0.45">
+    <row r="1" spans="2:88" ht="16.3" customHeight="1" x14ac:dyDescent="0.45">
       <c r="C1" s="63"/>
       <c r="D1" s="63"/>
       <c r="E1" s="63"/>
@@ -4679,7 +5891,7 @@
       <c r="H1" s="63"/>
       <c r="I1" s="63"/>
     </row>
-    <row r="2" spans="2:45" ht="16.3" customHeight="1" x14ac:dyDescent="0.45">
+    <row r="2" spans="2:88" ht="16.3" customHeight="1" x14ac:dyDescent="0.45">
       <c r="B2" s="64"/>
       <c r="C2" s="75"/>
       <c r="D2" s="75"/>
@@ -4690,7 +5902,7 @@
       <c r="I2" s="76"/>
       <c r="J2" s="65"/>
     </row>
-    <row r="3" spans="2:45" ht="16.3" customHeight="1" x14ac:dyDescent="0.45">
+    <row r="3" spans="2:88" ht="16.3" customHeight="1" x14ac:dyDescent="0.45">
       <c r="B3" s="64"/>
       <c r="C3" s="73">
         <v>43</v>
@@ -4715,7 +5927,7 @@
       </c>
       <c r="J3" s="65"/>
     </row>
-    <row r="4" spans="2:45" ht="16.3" customHeight="1" x14ac:dyDescent="0.45">
+    <row r="4" spans="2:88" ht="16.3" customHeight="1" x14ac:dyDescent="0.45">
       <c r="B4" s="64"/>
       <c r="C4" s="73">
         <v>36</v>
@@ -4740,7 +5952,7 @@
       </c>
       <c r="J4" s="65"/>
     </row>
-    <row r="5" spans="2:45" ht="16.3" customHeight="1" x14ac:dyDescent="0.45">
+    <row r="5" spans="2:88" ht="16.3" customHeight="1" x14ac:dyDescent="0.45">
       <c r="B5" s="64"/>
       <c r="C5" s="73">
         <v>29</v>
@@ -4765,7 +5977,7 @@
       </c>
       <c r="J5" s="65"/>
     </row>
-    <row r="6" spans="2:45" ht="16.3" customHeight="1" x14ac:dyDescent="0.45">
+    <row r="6" spans="2:88" ht="16.3" customHeight="1" x14ac:dyDescent="0.45">
       <c r="B6" s="64"/>
       <c r="C6" s="73">
         <v>22</v>
@@ -4790,7 +6002,7 @@
       </c>
       <c r="J6" s="65"/>
     </row>
-    <row r="7" spans="2:45" x14ac:dyDescent="0.45">
+    <row r="7" spans="2:88" x14ac:dyDescent="0.45">
       <c r="B7" s="64"/>
       <c r="C7" s="73">
         <v>15</v>
@@ -4815,7 +6027,7 @@
       </c>
       <c r="J7" s="65"/>
     </row>
-    <row r="8" spans="2:45" ht="16.3" customHeight="1" x14ac:dyDescent="0.45">
+    <row r="8" spans="2:88" ht="16.3" customHeight="1" x14ac:dyDescent="0.45">
       <c r="B8" s="64"/>
       <c r="C8" s="73">
         <v>8</v>
@@ -4842,7 +6054,7 @@
       <c r="O8" s="66"/>
       <c r="V8" s="66"/>
     </row>
-    <row r="9" spans="2:45" ht="16.3" customHeight="1" x14ac:dyDescent="0.45">
+    <row r="9" spans="2:88" ht="16.3" customHeight="1" x14ac:dyDescent="0.45">
       <c r="B9" s="64"/>
       <c r="C9" s="73">
         <v>1</v>
@@ -4878,7 +6090,7 @@
       <c r="W9" s="68"/>
       <c r="X9" s="68"/>
     </row>
-    <row r="10" spans="2:45" ht="16.3" customHeight="1" x14ac:dyDescent="0.45">
+    <row r="10" spans="2:88" ht="16.3" customHeight="1" x14ac:dyDescent="0.45">
       <c r="C10" s="69"/>
       <c r="D10" s="69"/>
       <c r="E10" s="69"/>
@@ -4899,7 +6111,7 @@
       <c r="W10" s="68"/>
       <c r="X10" s="68"/>
     </row>
-    <row r="11" spans="2:45" ht="16.3" customHeight="1" x14ac:dyDescent="0.45">
+    <row r="11" spans="2:88" ht="16.3" customHeight="1" x14ac:dyDescent="0.45">
       <c r="C11" s="68"/>
       <c r="D11" s="68"/>
       <c r="E11" s="68"/>
@@ -4919,7 +6131,7 @@
       <c r="W11" s="68"/>
       <c r="X11" s="68"/>
     </row>
-    <row r="12" spans="2:45" ht="16.3" customHeight="1" x14ac:dyDescent="0.45">
+    <row r="12" spans="2:88" ht="16.3" customHeight="1" x14ac:dyDescent="0.45">
       <c r="C12" s="78" t="s">
         <v>0</v>
       </c>
@@ -4948,8 +6160,20 @@
       <c r="AM12" s="79" t="s">
         <v>4</v>
       </c>
-    </row>
-    <row r="13" spans="2:45" ht="16.3" customHeight="1" x14ac:dyDescent="0.45">
+      <c r="AY12" s="79" t="s">
+        <v>25</v>
+      </c>
+      <c r="BI12" s="79" t="s">
+        <v>26</v>
+      </c>
+      <c r="BS12" s="79" t="s">
+        <v>27</v>
+      </c>
+      <c r="CC12" s="79" t="s">
+        <v>28</v>
+      </c>
+    </row>
+    <row r="13" spans="2:88" ht="16.3" customHeight="1" x14ac:dyDescent="0.45">
       <c r="C13" s="73">
         <v>43</v>
       </c>
@@ -5058,8 +6282,92 @@
       <c r="AS13" s="73">
         <v>49</v>
       </c>
-    </row>
-    <row r="14" spans="2:45" ht="16.3" customHeight="1" x14ac:dyDescent="0.45">
+      <c r="AY13" s="73">
+        <v>43</v>
+      </c>
+      <c r="AZ13" s="73">
+        <v>44</v>
+      </c>
+      <c r="BA13" s="73">
+        <v>45</v>
+      </c>
+      <c r="BB13" s="73">
+        <v>46</v>
+      </c>
+      <c r="BC13" s="73">
+        <v>47</v>
+      </c>
+      <c r="BD13" s="73">
+        <v>48</v>
+      </c>
+      <c r="BE13" s="73">
+        <v>49</v>
+      </c>
+      <c r="BI13" s="73">
+        <v>43</v>
+      </c>
+      <c r="BJ13" s="73">
+        <v>44</v>
+      </c>
+      <c r="BK13" s="73">
+        <v>45</v>
+      </c>
+      <c r="BL13" s="73">
+        <v>46</v>
+      </c>
+      <c r="BM13" s="73">
+        <v>47</v>
+      </c>
+      <c r="BN13" s="73">
+        <v>48</v>
+      </c>
+      <c r="BO13" s="73">
+        <v>49</v>
+      </c>
+      <c r="BS13" s="73">
+        <v>43</v>
+      </c>
+      <c r="BT13" s="73">
+        <v>44</v>
+      </c>
+      <c r="BU13" s="73">
+        <v>45</v>
+      </c>
+      <c r="BV13" s="73">
+        <v>46</v>
+      </c>
+      <c r="BW13" s="73">
+        <v>47</v>
+      </c>
+      <c r="BX13" s="73">
+        <v>48</v>
+      </c>
+      <c r="BY13" s="73">
+        <v>49</v>
+      </c>
+      <c r="CC13" s="73">
+        <v>43</v>
+      </c>
+      <c r="CD13" s="73">
+        <v>44</v>
+      </c>
+      <c r="CE13" s="73">
+        <v>45</v>
+      </c>
+      <c r="CF13" s="73">
+        <v>46</v>
+      </c>
+      <c r="CG13" s="73">
+        <v>47</v>
+      </c>
+      <c r="CH13" s="73">
+        <v>48</v>
+      </c>
+      <c r="CI13" s="73">
+        <v>49</v>
+      </c>
+    </row>
+    <row r="14" spans="2:88" ht="16.3" customHeight="1" x14ac:dyDescent="0.45">
       <c r="C14" s="73">
         <v>36</v>
       </c>
@@ -5165,8 +6473,92 @@
       <c r="AS14" s="74">
         <v>42</v>
       </c>
-    </row>
-    <row r="15" spans="2:45" ht="16.3" customHeight="1" x14ac:dyDescent="0.45">
+      <c r="AY14" s="73">
+        <v>36</v>
+      </c>
+      <c r="AZ14" s="77">
+        <v>37</v>
+      </c>
+      <c r="BA14" s="77">
+        <v>38</v>
+      </c>
+      <c r="BB14" s="77">
+        <v>39</v>
+      </c>
+      <c r="BC14" s="77">
+        <v>40</v>
+      </c>
+      <c r="BD14" s="77">
+        <v>41</v>
+      </c>
+      <c r="BE14" s="74">
+        <v>42</v>
+      </c>
+      <c r="BI14" s="73">
+        <v>36</v>
+      </c>
+      <c r="BJ14" s="77">
+        <v>37</v>
+      </c>
+      <c r="BK14" s="77">
+        <v>38</v>
+      </c>
+      <c r="BL14" s="77">
+        <v>39</v>
+      </c>
+      <c r="BM14" s="77">
+        <v>40</v>
+      </c>
+      <c r="BN14" s="77">
+        <v>41</v>
+      </c>
+      <c r="BO14" s="74">
+        <v>42</v>
+      </c>
+      <c r="BS14" s="73">
+        <v>36</v>
+      </c>
+      <c r="BT14" s="77">
+        <v>37</v>
+      </c>
+      <c r="BU14" s="77">
+        <v>38</v>
+      </c>
+      <c r="BV14" s="77">
+        <v>39</v>
+      </c>
+      <c r="BW14" s="77">
+        <v>40</v>
+      </c>
+      <c r="BX14" s="77">
+        <v>41</v>
+      </c>
+      <c r="BY14" s="74">
+        <v>42</v>
+      </c>
+      <c r="CC14" s="73">
+        <v>36</v>
+      </c>
+      <c r="CD14" s="77">
+        <v>37</v>
+      </c>
+      <c r="CE14" s="77">
+        <v>38</v>
+      </c>
+      <c r="CF14" s="77">
+        <v>39</v>
+      </c>
+      <c r="CG14" s="77">
+        <v>40</v>
+      </c>
+      <c r="CH14" s="77">
+        <v>41</v>
+      </c>
+      <c r="CI14" s="74">
+        <v>42</v>
+      </c>
+    </row>
+    <row r="15" spans="2:88" ht="16.3" customHeight="1" thickBot="1" x14ac:dyDescent="0.5">
       <c r="C15" s="73">
         <v>29</v>
       </c>
@@ -5275,8 +6667,92 @@
       <c r="AS15" s="73">
         <v>35</v>
       </c>
-    </row>
-    <row r="16" spans="2:45" ht="16.3" customHeight="1" thickBot="1" x14ac:dyDescent="0.5">
+      <c r="AY15" s="82">
+        <v>29</v>
+      </c>
+      <c r="AZ15" s="82">
+        <v>30</v>
+      </c>
+      <c r="BA15" s="82">
+        <v>31</v>
+      </c>
+      <c r="BB15" s="82">
+        <v>32</v>
+      </c>
+      <c r="BC15" s="73">
+        <v>33</v>
+      </c>
+      <c r="BD15" s="73">
+        <v>34</v>
+      </c>
+      <c r="BE15" s="73">
+        <v>35</v>
+      </c>
+      <c r="BI15" s="73">
+        <v>29</v>
+      </c>
+      <c r="BJ15" s="82">
+        <v>30</v>
+      </c>
+      <c r="BK15" s="82">
+        <v>31</v>
+      </c>
+      <c r="BL15" s="82">
+        <v>32</v>
+      </c>
+      <c r="BM15" s="82">
+        <v>33</v>
+      </c>
+      <c r="BN15" s="73">
+        <v>34</v>
+      </c>
+      <c r="BO15" s="73">
+        <v>35</v>
+      </c>
+      <c r="BS15" s="73">
+        <v>29</v>
+      </c>
+      <c r="BT15" s="73">
+        <v>30</v>
+      </c>
+      <c r="BU15" s="82">
+        <v>31</v>
+      </c>
+      <c r="BV15" s="82">
+        <v>32</v>
+      </c>
+      <c r="BW15" s="82">
+        <v>33</v>
+      </c>
+      <c r="BX15" s="82">
+        <v>34</v>
+      </c>
+      <c r="BY15" s="73">
+        <v>35</v>
+      </c>
+      <c r="CC15" s="73">
+        <v>29</v>
+      </c>
+      <c r="CD15" s="73">
+        <v>30</v>
+      </c>
+      <c r="CE15" s="73">
+        <v>31</v>
+      </c>
+      <c r="CF15" s="82">
+        <v>32</v>
+      </c>
+      <c r="CG15" s="82">
+        <v>33</v>
+      </c>
+      <c r="CH15" s="82">
+        <v>34</v>
+      </c>
+      <c r="CI15" s="82">
+        <v>35</v>
+      </c>
+    </row>
+    <row r="16" spans="2:88" ht="16.3" customHeight="1" thickTop="1" thickBot="1" x14ac:dyDescent="0.5">
       <c r="C16" s="82">
         <v>22</v>
       </c>
@@ -5385,8 +6861,94 @@
       <c r="AS16" s="98">
         <v>28</v>
       </c>
-    </row>
-    <row r="17" spans="2:46" ht="16.3" customHeight="1" thickTop="1" x14ac:dyDescent="0.45">
+      <c r="AX16" s="64"/>
+      <c r="AY16" s="85">
+        <v>22</v>
+      </c>
+      <c r="AZ16" s="101">
+        <v>23</v>
+      </c>
+      <c r="BA16" s="101">
+        <v>24</v>
+      </c>
+      <c r="BB16" s="102">
+        <v>25</v>
+      </c>
+      <c r="BC16" s="81">
+        <v>26</v>
+      </c>
+      <c r="BD16" s="77">
+        <v>27</v>
+      </c>
+      <c r="BE16" s="74">
+        <v>28</v>
+      </c>
+      <c r="BI16" s="94">
+        <v>22</v>
+      </c>
+      <c r="BJ16" s="105">
+        <v>23</v>
+      </c>
+      <c r="BK16" s="101">
+        <v>24</v>
+      </c>
+      <c r="BL16" s="101">
+        <v>25</v>
+      </c>
+      <c r="BM16" s="102">
+        <v>26</v>
+      </c>
+      <c r="BN16" s="81">
+        <v>27</v>
+      </c>
+      <c r="BO16" s="74">
+        <v>28</v>
+      </c>
+      <c r="BS16" s="73">
+        <v>22</v>
+      </c>
+      <c r="BT16" s="97">
+        <v>23</v>
+      </c>
+      <c r="BU16" s="105">
+        <v>24</v>
+      </c>
+      <c r="BV16" s="101">
+        <v>25</v>
+      </c>
+      <c r="BW16" s="101">
+        <v>26</v>
+      </c>
+      <c r="BX16" s="102">
+        <v>27</v>
+      </c>
+      <c r="BY16" s="95">
+        <v>28</v>
+      </c>
+      <c r="CC16" s="73">
+        <v>22</v>
+      </c>
+      <c r="CD16" s="77">
+        <v>23</v>
+      </c>
+      <c r="CE16" s="97">
+        <v>24</v>
+      </c>
+      <c r="CF16" s="105">
+        <v>25</v>
+      </c>
+      <c r="CG16" s="101">
+        <v>26</v>
+      </c>
+      <c r="CH16" s="101">
+        <v>27</v>
+      </c>
+      <c r="CI16" s="107">
+        <v>28</v>
+      </c>
+      <c r="CJ16" s="65"/>
+    </row>
+    <row r="17" spans="2:88" ht="16.3" customHeight="1" thickTop="1" x14ac:dyDescent="0.45">
       <c r="B17" s="64"/>
       <c r="C17" s="85">
         <v>15</v>
@@ -5497,8 +7059,94 @@
         <v>21</v>
       </c>
       <c r="AT17" s="65"/>
-    </row>
-    <row r="18" spans="2:46" ht="16.3" customHeight="1" x14ac:dyDescent="0.45">
+      <c r="AX17" s="64"/>
+      <c r="AY17" s="88">
+        <v>15</v>
+      </c>
+      <c r="AZ17" s="73">
+        <v>16</v>
+      </c>
+      <c r="BA17" s="73">
+        <v>17</v>
+      </c>
+      <c r="BB17" s="90">
+        <v>18</v>
+      </c>
+      <c r="BC17" s="80">
+        <v>19</v>
+      </c>
+      <c r="BD17" s="73">
+        <v>20</v>
+      </c>
+      <c r="BE17" s="73">
+        <v>21</v>
+      </c>
+      <c r="BI17" s="94">
+        <v>15</v>
+      </c>
+      <c r="BJ17" s="88">
+        <v>16</v>
+      </c>
+      <c r="BK17" s="73">
+        <v>17</v>
+      </c>
+      <c r="BL17" s="73">
+        <v>18</v>
+      </c>
+      <c r="BM17" s="90">
+        <v>19</v>
+      </c>
+      <c r="BN17" s="80">
+        <v>20</v>
+      </c>
+      <c r="BO17" s="73">
+        <v>21</v>
+      </c>
+      <c r="BS17" s="73">
+        <v>15</v>
+      </c>
+      <c r="BT17" s="94">
+        <v>16</v>
+      </c>
+      <c r="BU17" s="88">
+        <v>17</v>
+      </c>
+      <c r="BV17" s="73">
+        <v>18</v>
+      </c>
+      <c r="BW17" s="73">
+        <v>19</v>
+      </c>
+      <c r="BX17" s="90">
+        <v>20</v>
+      </c>
+      <c r="BY17" s="80">
+        <v>21</v>
+      </c>
+      <c r="CC17" s="73">
+        <v>15</v>
+      </c>
+      <c r="CD17" s="73">
+        <v>16</v>
+      </c>
+      <c r="CE17" s="94">
+        <v>17</v>
+      </c>
+      <c r="CF17" s="88">
+        <v>18</v>
+      </c>
+      <c r="CG17" s="73">
+        <v>19</v>
+      </c>
+      <c r="CH17" s="73">
+        <v>20</v>
+      </c>
+      <c r="CI17" s="90">
+        <v>21</v>
+      </c>
+      <c r="CJ17" s="65"/>
+    </row>
+    <row r="18" spans="2:88" ht="16.3" customHeight="1" x14ac:dyDescent="0.45">
       <c r="B18" s="64"/>
       <c r="C18" s="88">
         <v>8</v>
@@ -5609,8 +7257,94 @@
         <v>14</v>
       </c>
       <c r="AT18" s="65"/>
-    </row>
-    <row r="19" spans="2:46" ht="16.3" customHeight="1" thickBot="1" x14ac:dyDescent="0.5">
+      <c r="AX18" s="64"/>
+      <c r="AY18" s="88">
+        <v>8</v>
+      </c>
+      <c r="AZ18" s="77">
+        <v>9</v>
+      </c>
+      <c r="BA18" s="77">
+        <v>10</v>
+      </c>
+      <c r="BB18" s="89">
+        <v>11</v>
+      </c>
+      <c r="BC18" s="81">
+        <v>12</v>
+      </c>
+      <c r="BD18" s="77">
+        <v>13</v>
+      </c>
+      <c r="BE18" s="74">
+        <v>14</v>
+      </c>
+      <c r="BI18" s="94">
+        <v>8</v>
+      </c>
+      <c r="BJ18" s="96">
+        <v>9</v>
+      </c>
+      <c r="BK18" s="77">
+        <v>10</v>
+      </c>
+      <c r="BL18" s="77">
+        <v>11</v>
+      </c>
+      <c r="BM18" s="89">
+        <v>12</v>
+      </c>
+      <c r="BN18" s="81">
+        <v>13</v>
+      </c>
+      <c r="BO18" s="74">
+        <v>14</v>
+      </c>
+      <c r="BS18" s="73">
+        <v>8</v>
+      </c>
+      <c r="BT18" s="97">
+        <v>9</v>
+      </c>
+      <c r="BU18" s="96">
+        <v>10</v>
+      </c>
+      <c r="BV18" s="77">
+        <v>11</v>
+      </c>
+      <c r="BW18" s="77">
+        <v>12</v>
+      </c>
+      <c r="BX18" s="89">
+        <v>13</v>
+      </c>
+      <c r="BY18" s="95">
+        <v>14</v>
+      </c>
+      <c r="CC18" s="73">
+        <v>8</v>
+      </c>
+      <c r="CD18" s="77">
+        <v>9</v>
+      </c>
+      <c r="CE18" s="97">
+        <v>10</v>
+      </c>
+      <c r="CF18" s="96">
+        <v>11</v>
+      </c>
+      <c r="CG18" s="77">
+        <v>12</v>
+      </c>
+      <c r="CH18" s="77">
+        <v>13</v>
+      </c>
+      <c r="CI18" s="99">
+        <v>14</v>
+      </c>
+      <c r="CJ18" s="65"/>
+    </row>
+    <row r="19" spans="2:88" ht="16.3" customHeight="1" thickBot="1" x14ac:dyDescent="0.5">
       <c r="B19" s="64"/>
       <c r="C19" s="91">
         <v>1</v>
@@ -5721,8 +7455,94 @@
         <v>7</v>
       </c>
       <c r="AT19" s="65"/>
-    </row>
-    <row r="20" spans="2:46" ht="16.3" customHeight="1" thickTop="1" x14ac:dyDescent="0.45">
+      <c r="AX19" s="64"/>
+      <c r="AY19" s="91">
+        <v>1</v>
+      </c>
+      <c r="AZ19" s="92">
+        <v>2</v>
+      </c>
+      <c r="BA19" s="92">
+        <v>3</v>
+      </c>
+      <c r="BB19" s="93">
+        <v>4</v>
+      </c>
+      <c r="BC19" s="80">
+        <v>5</v>
+      </c>
+      <c r="BD19" s="73">
+        <v>6</v>
+      </c>
+      <c r="BE19" s="73">
+        <v>7</v>
+      </c>
+      <c r="BI19" s="94">
+        <v>1</v>
+      </c>
+      <c r="BJ19" s="91">
+        <v>2</v>
+      </c>
+      <c r="BK19" s="92">
+        <v>3</v>
+      </c>
+      <c r="BL19" s="92">
+        <v>4</v>
+      </c>
+      <c r="BM19" s="93">
+        <v>5</v>
+      </c>
+      <c r="BN19" s="80">
+        <v>6</v>
+      </c>
+      <c r="BO19" s="73">
+        <v>7</v>
+      </c>
+      <c r="BS19" s="73">
+        <v>1</v>
+      </c>
+      <c r="BT19" s="94">
+        <v>2</v>
+      </c>
+      <c r="BU19" s="91">
+        <v>3</v>
+      </c>
+      <c r="BV19" s="92">
+        <v>4</v>
+      </c>
+      <c r="BW19" s="92">
+        <v>5</v>
+      </c>
+      <c r="BX19" s="93">
+        <v>6</v>
+      </c>
+      <c r="BY19" s="80">
+        <v>7</v>
+      </c>
+      <c r="CC19" s="73">
+        <v>1</v>
+      </c>
+      <c r="CD19" s="73">
+        <v>2</v>
+      </c>
+      <c r="CE19" s="94">
+        <v>3</v>
+      </c>
+      <c r="CF19" s="91">
+        <v>4</v>
+      </c>
+      <c r="CG19" s="92">
+        <v>5</v>
+      </c>
+      <c r="CH19" s="92">
+        <v>6</v>
+      </c>
+      <c r="CI19" s="93">
+        <v>7</v>
+      </c>
+      <c r="CJ19" s="65"/>
+    </row>
+    <row r="20" spans="2:88" ht="16.3" customHeight="1" thickTop="1" x14ac:dyDescent="0.45">
       <c r="C20" s="84"/>
       <c r="D20" s="70"/>
       <c r="E20" s="70"/>
@@ -5739,8 +7559,24 @@
       <c r="AQ20" s="70"/>
       <c r="AR20" s="70"/>
       <c r="AS20" s="70"/>
-    </row>
-    <row r="21" spans="2:46" ht="16.3" customHeight="1" x14ac:dyDescent="0.45">
+      <c r="AY20" s="70"/>
+      <c r="AZ20" s="70"/>
+      <c r="BA20" s="70"/>
+      <c r="BB20" s="70"/>
+      <c r="BJ20" s="70"/>
+      <c r="BK20" s="70"/>
+      <c r="BL20" s="70"/>
+      <c r="BM20" s="70"/>
+      <c r="BU20" s="70"/>
+      <c r="BV20" s="70"/>
+      <c r="BW20" s="70"/>
+      <c r="BX20" s="70"/>
+      <c r="CF20" s="70"/>
+      <c r="CG20" s="70"/>
+      <c r="CH20" s="70"/>
+      <c r="CI20" s="70"/>
+    </row>
+    <row r="21" spans="2:88" ht="16.3" customHeight="1" x14ac:dyDescent="0.45">
       <c r="C21" s="78" t="s">
         <v>5</v>
       </c>
@@ -5769,8 +7605,20 @@
       <c r="AM21" s="79" t="s">
         <v>9</v>
       </c>
-    </row>
-    <row r="22" spans="2:46" ht="16.3" customHeight="1" x14ac:dyDescent="0.45">
+      <c r="AY21" s="79" t="s">
+        <v>29</v>
+      </c>
+      <c r="BI21" s="79" t="s">
+        <v>30</v>
+      </c>
+      <c r="BS21" s="79" t="s">
+        <v>31</v>
+      </c>
+      <c r="CC21" s="79" t="s">
+        <v>32</v>
+      </c>
+    </row>
+    <row r="22" spans="2:88" ht="16.3" customHeight="1" x14ac:dyDescent="0.45">
       <c r="C22" s="73">
         <v>43</v>
       </c>
@@ -5879,8 +7727,92 @@
       <c r="AS22" s="73">
         <v>49</v>
       </c>
-    </row>
-    <row r="23" spans="2:46" ht="16.3" customHeight="1" x14ac:dyDescent="0.45">
+      <c r="AY22" s="73">
+        <v>43</v>
+      </c>
+      <c r="AZ22" s="73">
+        <v>44</v>
+      </c>
+      <c r="BA22" s="73">
+        <v>45</v>
+      </c>
+      <c r="BB22" s="73">
+        <v>46</v>
+      </c>
+      <c r="BC22" s="73">
+        <v>47</v>
+      </c>
+      <c r="BD22" s="73">
+        <v>48</v>
+      </c>
+      <c r="BE22" s="73">
+        <v>49</v>
+      </c>
+      <c r="BI22" s="73">
+        <v>43</v>
+      </c>
+      <c r="BJ22" s="73">
+        <v>44</v>
+      </c>
+      <c r="BK22" s="73">
+        <v>45</v>
+      </c>
+      <c r="BL22" s="73">
+        <v>46</v>
+      </c>
+      <c r="BM22" s="73">
+        <v>47</v>
+      </c>
+      <c r="BN22" s="73">
+        <v>48</v>
+      </c>
+      <c r="BO22" s="73">
+        <v>49</v>
+      </c>
+      <c r="BS22" s="73">
+        <v>43</v>
+      </c>
+      <c r="BT22" s="73">
+        <v>44</v>
+      </c>
+      <c r="BU22" s="73">
+        <v>45</v>
+      </c>
+      <c r="BV22" s="73">
+        <v>46</v>
+      </c>
+      <c r="BW22" s="73">
+        <v>47</v>
+      </c>
+      <c r="BX22" s="73">
+        <v>48</v>
+      </c>
+      <c r="BY22" s="73">
+        <v>49</v>
+      </c>
+      <c r="CC22" s="73">
+        <v>43</v>
+      </c>
+      <c r="CD22" s="73">
+        <v>44</v>
+      </c>
+      <c r="CE22" s="73">
+        <v>45</v>
+      </c>
+      <c r="CF22" s="73">
+        <v>46</v>
+      </c>
+      <c r="CG22" s="73">
+        <v>47</v>
+      </c>
+      <c r="CH22" s="73">
+        <v>48</v>
+      </c>
+      <c r="CI22" s="73">
+        <v>49</v>
+      </c>
+    </row>
+    <row r="23" spans="2:88" ht="16.3" customHeight="1" thickBot="1" x14ac:dyDescent="0.5">
       <c r="C23" s="73">
         <v>36</v>
       </c>
@@ -5989,8 +7921,92 @@
       <c r="AS23" s="74">
         <v>42</v>
       </c>
-    </row>
-    <row r="24" spans="2:46" ht="16.3" customHeight="1" thickBot="1" x14ac:dyDescent="0.5">
+      <c r="AY23" s="82">
+        <v>36</v>
+      </c>
+      <c r="AZ23" s="83">
+        <v>37</v>
+      </c>
+      <c r="BA23" s="83">
+        <v>38</v>
+      </c>
+      <c r="BB23" s="83">
+        <v>39</v>
+      </c>
+      <c r="BC23" s="77">
+        <v>40</v>
+      </c>
+      <c r="BD23" s="77">
+        <v>41</v>
+      </c>
+      <c r="BE23" s="74">
+        <v>42</v>
+      </c>
+      <c r="BI23" s="73">
+        <v>36</v>
+      </c>
+      <c r="BJ23" s="83">
+        <v>37</v>
+      </c>
+      <c r="BK23" s="83">
+        <v>38</v>
+      </c>
+      <c r="BL23" s="83">
+        <v>39</v>
+      </c>
+      <c r="BM23" s="83">
+        <v>40</v>
+      </c>
+      <c r="BN23" s="77">
+        <v>41</v>
+      </c>
+      <c r="BO23" s="74">
+        <v>42</v>
+      </c>
+      <c r="BS23" s="73">
+        <v>36</v>
+      </c>
+      <c r="BT23" s="77">
+        <v>37</v>
+      </c>
+      <c r="BU23" s="83">
+        <v>38</v>
+      </c>
+      <c r="BV23" s="83">
+        <v>39</v>
+      </c>
+      <c r="BW23" s="83">
+        <v>40</v>
+      </c>
+      <c r="BX23" s="83">
+        <v>41</v>
+      </c>
+      <c r="BY23" s="74">
+        <v>42</v>
+      </c>
+      <c r="CC23" s="73">
+        <v>36</v>
+      </c>
+      <c r="CD23" s="77">
+        <v>37</v>
+      </c>
+      <c r="CE23" s="77">
+        <v>38</v>
+      </c>
+      <c r="CF23" s="83">
+        <v>39</v>
+      </c>
+      <c r="CG23" s="83">
+        <v>40</v>
+      </c>
+      <c r="CH23" s="83">
+        <v>41</v>
+      </c>
+      <c r="CI23" s="98">
+        <v>42</v>
+      </c>
+    </row>
+    <row r="24" spans="2:88" ht="16.3" customHeight="1" thickTop="1" thickBot="1" x14ac:dyDescent="0.5">
       <c r="C24" s="82">
         <v>29</v>
       </c>
@@ -6099,8 +8115,94 @@
       <c r="AS24" s="82">
         <v>35</v>
       </c>
-    </row>
-    <row r="25" spans="2:46" ht="16.3" customHeight="1" thickTop="1" x14ac:dyDescent="0.45">
+      <c r="AX24" s="64"/>
+      <c r="AY24" s="85">
+        <v>29</v>
+      </c>
+      <c r="AZ24" s="86">
+        <v>30</v>
+      </c>
+      <c r="BA24" s="86">
+        <v>31</v>
+      </c>
+      <c r="BB24" s="87">
+        <v>32</v>
+      </c>
+      <c r="BC24" s="80">
+        <v>33</v>
+      </c>
+      <c r="BD24" s="73">
+        <v>34</v>
+      </c>
+      <c r="BE24" s="73">
+        <v>35</v>
+      </c>
+      <c r="BI24" s="94">
+        <v>29</v>
+      </c>
+      <c r="BJ24" s="85">
+        <v>30</v>
+      </c>
+      <c r="BK24" s="86">
+        <v>31</v>
+      </c>
+      <c r="BL24" s="86">
+        <v>32</v>
+      </c>
+      <c r="BM24" s="87">
+        <v>33</v>
+      </c>
+      <c r="BN24" s="80">
+        <v>34</v>
+      </c>
+      <c r="BO24" s="73">
+        <v>35</v>
+      </c>
+      <c r="BS24" s="73">
+        <v>29</v>
+      </c>
+      <c r="BT24" s="94">
+        <v>30</v>
+      </c>
+      <c r="BU24" s="85">
+        <v>31</v>
+      </c>
+      <c r="BV24" s="86">
+        <v>32</v>
+      </c>
+      <c r="BW24" s="86">
+        <v>33</v>
+      </c>
+      <c r="BX24" s="87">
+        <v>34</v>
+      </c>
+      <c r="BY24" s="80">
+        <v>35</v>
+      </c>
+      <c r="CC24" s="73">
+        <v>29</v>
+      </c>
+      <c r="CD24" s="73">
+        <v>30</v>
+      </c>
+      <c r="CE24" s="94">
+        <v>31</v>
+      </c>
+      <c r="CF24" s="85">
+        <v>32</v>
+      </c>
+      <c r="CG24" s="86">
+        <v>33</v>
+      </c>
+      <c r="CH24" s="86">
+        <v>34</v>
+      </c>
+      <c r="CI24" s="87">
+        <v>35</v>
+      </c>
+      <c r="CJ24" s="65"/>
+    </row>
+    <row r="25" spans="2:88" ht="16.3" customHeight="1" thickTop="1" x14ac:dyDescent="0.45">
       <c r="B25" s="64"/>
       <c r="C25" s="85">
         <v>22</v>
@@ -6211,8 +8313,94 @@
         <v>28</v>
       </c>
       <c r="AT25" s="65"/>
-    </row>
-    <row r="26" spans="2:46" x14ac:dyDescent="0.45">
+      <c r="AX25" s="64"/>
+      <c r="AY25" s="88">
+        <v>22</v>
+      </c>
+      <c r="AZ25" s="77">
+        <v>23</v>
+      </c>
+      <c r="BA25" s="77">
+        <v>24</v>
+      </c>
+      <c r="BB25" s="89">
+        <v>25</v>
+      </c>
+      <c r="BC25" s="81">
+        <v>26</v>
+      </c>
+      <c r="BD25" s="77">
+        <v>27</v>
+      </c>
+      <c r="BE25" s="74">
+        <v>28</v>
+      </c>
+      <c r="BI25" s="94">
+        <v>22</v>
+      </c>
+      <c r="BJ25" s="96">
+        <v>23</v>
+      </c>
+      <c r="BK25" s="77">
+        <v>24</v>
+      </c>
+      <c r="BL25" s="77">
+        <v>25</v>
+      </c>
+      <c r="BM25" s="89">
+        <v>26</v>
+      </c>
+      <c r="BN25" s="81">
+        <v>27</v>
+      </c>
+      <c r="BO25" s="74">
+        <v>28</v>
+      </c>
+      <c r="BS25" s="73">
+        <v>22</v>
+      </c>
+      <c r="BT25" s="97">
+        <v>23</v>
+      </c>
+      <c r="BU25" s="96">
+        <v>24</v>
+      </c>
+      <c r="BV25" s="77">
+        <v>25</v>
+      </c>
+      <c r="BW25" s="77">
+        <v>26</v>
+      </c>
+      <c r="BX25" s="89">
+        <v>27</v>
+      </c>
+      <c r="BY25" s="95">
+        <v>28</v>
+      </c>
+      <c r="CC25" s="73">
+        <v>22</v>
+      </c>
+      <c r="CD25" s="77">
+        <v>23</v>
+      </c>
+      <c r="CE25" s="97">
+        <v>24</v>
+      </c>
+      <c r="CF25" s="96">
+        <v>25</v>
+      </c>
+      <c r="CG25" s="77">
+        <v>26</v>
+      </c>
+      <c r="CH25" s="77">
+        <v>27</v>
+      </c>
+      <c r="CI25" s="99">
+        <v>28</v>
+      </c>
+      <c r="CJ25" s="65"/>
+    </row>
+    <row r="26" spans="2:88" x14ac:dyDescent="0.45">
       <c r="B26" s="64"/>
       <c r="C26" s="88">
         <v>15</v>
@@ -6320,8 +8508,94 @@
         <v>21</v>
       </c>
       <c r="AT26" s="65"/>
-    </row>
-    <row r="27" spans="2:46" ht="16.3" customHeight="1" thickBot="1" x14ac:dyDescent="0.5">
+      <c r="AX26" s="64"/>
+      <c r="AY26" s="88">
+        <v>15</v>
+      </c>
+      <c r="AZ26" s="73">
+        <v>16</v>
+      </c>
+      <c r="BA26" s="73">
+        <v>17</v>
+      </c>
+      <c r="BB26" s="90">
+        <v>18</v>
+      </c>
+      <c r="BC26" s="80">
+        <v>19</v>
+      </c>
+      <c r="BD26" s="73">
+        <v>20</v>
+      </c>
+      <c r="BE26" s="73">
+        <v>21</v>
+      </c>
+      <c r="BI26" s="94">
+        <v>15</v>
+      </c>
+      <c r="BJ26" s="88">
+        <v>16</v>
+      </c>
+      <c r="BK26" s="73">
+        <v>17</v>
+      </c>
+      <c r="BL26" s="73">
+        <v>18</v>
+      </c>
+      <c r="BM26" s="90">
+        <v>19</v>
+      </c>
+      <c r="BN26" s="80">
+        <v>20</v>
+      </c>
+      <c r="BO26" s="73">
+        <v>21</v>
+      </c>
+      <c r="BS26" s="73">
+        <v>15</v>
+      </c>
+      <c r="BT26" s="94">
+        <v>16</v>
+      </c>
+      <c r="BU26" s="88">
+        <v>17</v>
+      </c>
+      <c r="BV26" s="73">
+        <v>18</v>
+      </c>
+      <c r="BW26" s="73">
+        <v>19</v>
+      </c>
+      <c r="BX26" s="90">
+        <v>20</v>
+      </c>
+      <c r="BY26" s="80">
+        <v>21</v>
+      </c>
+      <c r="CC26" s="73">
+        <v>15</v>
+      </c>
+      <c r="CD26" s="73">
+        <v>16</v>
+      </c>
+      <c r="CE26" s="94">
+        <v>17</v>
+      </c>
+      <c r="CF26" s="88">
+        <v>18</v>
+      </c>
+      <c r="CG26" s="73">
+        <v>19</v>
+      </c>
+      <c r="CH26" s="73">
+        <v>20</v>
+      </c>
+      <c r="CI26" s="90">
+        <v>21</v>
+      </c>
+      <c r="CJ26" s="65"/>
+    </row>
+    <row r="27" spans="2:88" ht="16.3" customHeight="1" thickBot="1" x14ac:dyDescent="0.5">
       <c r="B27" s="64"/>
       <c r="C27" s="91">
         <v>8</v>
@@ -6429,8 +8703,94 @@
         <v>14</v>
       </c>
       <c r="AT27" s="65"/>
-    </row>
-    <row r="28" spans="2:46" ht="16.3" customHeight="1" thickTop="1" x14ac:dyDescent="0.45">
+      <c r="AX27" s="64"/>
+      <c r="AY27" s="91">
+        <v>8</v>
+      </c>
+      <c r="AZ27" s="103">
+        <v>9</v>
+      </c>
+      <c r="BA27" s="103">
+        <v>10</v>
+      </c>
+      <c r="BB27" s="104">
+        <v>11</v>
+      </c>
+      <c r="BC27" s="81">
+        <v>12</v>
+      </c>
+      <c r="BD27" s="77">
+        <v>13</v>
+      </c>
+      <c r="BE27" s="74">
+        <v>14</v>
+      </c>
+      <c r="BI27" s="94">
+        <v>8</v>
+      </c>
+      <c r="BJ27" s="106">
+        <v>9</v>
+      </c>
+      <c r="BK27" s="103">
+        <v>10</v>
+      </c>
+      <c r="BL27" s="103">
+        <v>11</v>
+      </c>
+      <c r="BM27" s="104">
+        <v>12</v>
+      </c>
+      <c r="BN27" s="81">
+        <v>13</v>
+      </c>
+      <c r="BO27" s="74">
+        <v>14</v>
+      </c>
+      <c r="BS27" s="73">
+        <v>8</v>
+      </c>
+      <c r="BT27" s="97">
+        <v>9</v>
+      </c>
+      <c r="BU27" s="106">
+        <v>10</v>
+      </c>
+      <c r="BV27" s="103">
+        <v>11</v>
+      </c>
+      <c r="BW27" s="103">
+        <v>12</v>
+      </c>
+      <c r="BX27" s="104">
+        <v>13</v>
+      </c>
+      <c r="BY27" s="95">
+        <v>14</v>
+      </c>
+      <c r="CC27" s="73">
+        <v>8</v>
+      </c>
+      <c r="CD27" s="77">
+        <v>9</v>
+      </c>
+      <c r="CE27" s="97">
+        <v>10</v>
+      </c>
+      <c r="CF27" s="106">
+        <v>11</v>
+      </c>
+      <c r="CG27" s="103">
+        <v>12</v>
+      </c>
+      <c r="CH27" s="103">
+        <v>13</v>
+      </c>
+      <c r="CI27" s="108">
+        <v>14</v>
+      </c>
+      <c r="CJ27" s="65"/>
+    </row>
+    <row r="28" spans="2:88" ht="16.3" customHeight="1" thickTop="1" x14ac:dyDescent="0.45">
       <c r="C28" s="100">
         <v>1</v>
       </c>
@@ -6541,8 +8901,92 @@
       <c r="AS28" s="100">
         <v>7</v>
       </c>
-    </row>
-    <row r="29" spans="2:46" ht="16.3" customHeight="1" x14ac:dyDescent="0.45">
+      <c r="AY28" s="100">
+        <v>1</v>
+      </c>
+      <c r="AZ28" s="100">
+        <v>2</v>
+      </c>
+      <c r="BA28" s="100">
+        <v>3</v>
+      </c>
+      <c r="BB28" s="100">
+        <v>4</v>
+      </c>
+      <c r="BC28" s="73">
+        <v>5</v>
+      </c>
+      <c r="BD28" s="73">
+        <v>6</v>
+      </c>
+      <c r="BE28" s="73">
+        <v>7</v>
+      </c>
+      <c r="BI28" s="73">
+        <v>1</v>
+      </c>
+      <c r="BJ28" s="100">
+        <v>2</v>
+      </c>
+      <c r="BK28" s="100">
+        <v>3</v>
+      </c>
+      <c r="BL28" s="100">
+        <v>4</v>
+      </c>
+      <c r="BM28" s="100">
+        <v>5</v>
+      </c>
+      <c r="BN28" s="73">
+        <v>6</v>
+      </c>
+      <c r="BO28" s="73">
+        <v>7</v>
+      </c>
+      <c r="BS28" s="73">
+        <v>1</v>
+      </c>
+      <c r="BT28" s="73">
+        <v>2</v>
+      </c>
+      <c r="BU28" s="100">
+        <v>3</v>
+      </c>
+      <c r="BV28" s="100">
+        <v>4</v>
+      </c>
+      <c r="BW28" s="100">
+        <v>5</v>
+      </c>
+      <c r="BX28" s="100">
+        <v>6</v>
+      </c>
+      <c r="BY28" s="73">
+        <v>7</v>
+      </c>
+      <c r="CC28" s="73">
+        <v>1</v>
+      </c>
+      <c r="CD28" s="73">
+        <v>2</v>
+      </c>
+      <c r="CE28" s="73">
+        <v>3</v>
+      </c>
+      <c r="CF28" s="100">
+        <v>4</v>
+      </c>
+      <c r="CG28" s="100">
+        <v>5</v>
+      </c>
+      <c r="CH28" s="100">
+        <v>6</v>
+      </c>
+      <c r="CI28" s="100">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="29" spans="2:88" ht="16.3" customHeight="1" x14ac:dyDescent="0.45">
       <c r="C29" s="68"/>
       <c r="D29" s="68"/>
       <c r="E29" s="68"/>
@@ -6569,7 +9013,7 @@
       <c r="AD29" s="68"/>
       <c r="AE29" s="68"/>
     </row>
-    <row r="30" spans="2:46" ht="16.3" customHeight="1" x14ac:dyDescent="0.45">
+    <row r="30" spans="2:88" ht="16.3" customHeight="1" x14ac:dyDescent="0.45">
       <c r="C30" s="78" t="s">
         <v>10</v>
       </c>
@@ -6606,8 +9050,20 @@
       <c r="AM30" s="79" t="s">
         <v>14</v>
       </c>
-    </row>
-    <row r="31" spans="2:46" ht="16.3" customHeight="1" x14ac:dyDescent="0.45">
+      <c r="AY30" s="79" t="s">
+        <v>33</v>
+      </c>
+      <c r="BI30" s="79" t="s">
+        <v>34</v>
+      </c>
+      <c r="BS30" s="79" t="s">
+        <v>35</v>
+      </c>
+      <c r="CC30" s="79" t="s">
+        <v>36</v>
+      </c>
+    </row>
+    <row r="31" spans="2:88" ht="16.3" customHeight="1" thickBot="1" x14ac:dyDescent="0.5">
       <c r="C31" s="73">
         <v>43</v>
       </c>
@@ -6716,8 +9172,92 @@
       <c r="AS31" s="73">
         <v>49</v>
       </c>
-    </row>
-    <row r="32" spans="2:46" ht="16.3" customHeight="1" thickBot="1" x14ac:dyDescent="0.5">
+      <c r="AY31" s="82">
+        <v>43</v>
+      </c>
+      <c r="AZ31" s="82">
+        <v>44</v>
+      </c>
+      <c r="BA31" s="82">
+        <v>45</v>
+      </c>
+      <c r="BB31" s="82">
+        <v>46</v>
+      </c>
+      <c r="BC31" s="73">
+        <v>47</v>
+      </c>
+      <c r="BD31" s="73">
+        <v>48</v>
+      </c>
+      <c r="BE31" s="73">
+        <v>49</v>
+      </c>
+      <c r="BI31" s="73">
+        <v>43</v>
+      </c>
+      <c r="BJ31" s="82">
+        <v>44</v>
+      </c>
+      <c r="BK31" s="82">
+        <v>45</v>
+      </c>
+      <c r="BL31" s="82">
+        <v>46</v>
+      </c>
+      <c r="BM31" s="82">
+        <v>47</v>
+      </c>
+      <c r="BN31" s="73">
+        <v>48</v>
+      </c>
+      <c r="BO31" s="73">
+        <v>49</v>
+      </c>
+      <c r="BS31" s="73">
+        <v>43</v>
+      </c>
+      <c r="BT31" s="73">
+        <v>44</v>
+      </c>
+      <c r="BU31" s="82">
+        <v>45</v>
+      </c>
+      <c r="BV31" s="82">
+        <v>46</v>
+      </c>
+      <c r="BW31" s="82">
+        <v>47</v>
+      </c>
+      <c r="BX31" s="82">
+        <v>48</v>
+      </c>
+      <c r="BY31" s="73">
+        <v>49</v>
+      </c>
+      <c r="CC31" s="73">
+        <v>43</v>
+      </c>
+      <c r="CD31" s="73">
+        <v>44</v>
+      </c>
+      <c r="CE31" s="73">
+        <v>45</v>
+      </c>
+      <c r="CF31" s="82">
+        <v>46</v>
+      </c>
+      <c r="CG31" s="82">
+        <v>47</v>
+      </c>
+      <c r="CH31" s="82">
+        <v>48</v>
+      </c>
+      <c r="CI31" s="82">
+        <v>49</v>
+      </c>
+    </row>
+    <row r="32" spans="2:88" ht="16.3" customHeight="1" thickTop="1" thickBot="1" x14ac:dyDescent="0.5">
       <c r="C32" s="82">
         <v>36</v>
       </c>
@@ -6823,8 +9363,94 @@
       <c r="AS32" s="98">
         <v>42</v>
       </c>
-    </row>
-    <row r="33" spans="2:46" ht="15.6" thickTop="1" x14ac:dyDescent="0.45">
+      <c r="AX32" s="64"/>
+      <c r="AY32" s="85">
+        <v>36</v>
+      </c>
+      <c r="AZ32" s="101">
+        <v>37</v>
+      </c>
+      <c r="BA32" s="101">
+        <v>38</v>
+      </c>
+      <c r="BB32" s="102">
+        <v>39</v>
+      </c>
+      <c r="BC32" s="81">
+        <v>40</v>
+      </c>
+      <c r="BD32" s="77">
+        <v>41</v>
+      </c>
+      <c r="BE32" s="74">
+        <v>42</v>
+      </c>
+      <c r="BI32" s="94">
+        <v>36</v>
+      </c>
+      <c r="BJ32" s="105">
+        <v>37</v>
+      </c>
+      <c r="BK32" s="101">
+        <v>38</v>
+      </c>
+      <c r="BL32" s="101">
+        <v>39</v>
+      </c>
+      <c r="BM32" s="102">
+        <v>40</v>
+      </c>
+      <c r="BN32" s="81">
+        <v>41</v>
+      </c>
+      <c r="BO32" s="74">
+        <v>42</v>
+      </c>
+      <c r="BS32" s="73">
+        <v>36</v>
+      </c>
+      <c r="BT32" s="97">
+        <v>37</v>
+      </c>
+      <c r="BU32" s="105">
+        <v>38</v>
+      </c>
+      <c r="BV32" s="101">
+        <v>39</v>
+      </c>
+      <c r="BW32" s="101">
+        <v>40</v>
+      </c>
+      <c r="BX32" s="102">
+        <v>41</v>
+      </c>
+      <c r="BY32" s="95">
+        <v>42</v>
+      </c>
+      <c r="CC32" s="73">
+        <v>36</v>
+      </c>
+      <c r="CD32" s="77">
+        <v>37</v>
+      </c>
+      <c r="CE32" s="97">
+        <v>38</v>
+      </c>
+      <c r="CF32" s="105">
+        <v>39</v>
+      </c>
+      <c r="CG32" s="101">
+        <v>40</v>
+      </c>
+      <c r="CH32" s="101">
+        <v>41</v>
+      </c>
+      <c r="CI32" s="107">
+        <v>42</v>
+      </c>
+      <c r="CJ32" s="65"/>
+    </row>
+    <row r="33" spans="2:88" ht="15.6" thickTop="1" x14ac:dyDescent="0.45">
       <c r="B33" s="64"/>
       <c r="C33" s="85">
         <v>29</v>
@@ -6935,8 +9561,94 @@
         <v>35</v>
       </c>
       <c r="AT33" s="65"/>
-    </row>
-    <row r="34" spans="2:46" ht="16.3" customHeight="1" x14ac:dyDescent="0.45">
+      <c r="AX33" s="64"/>
+      <c r="AY33" s="88">
+        <v>29</v>
+      </c>
+      <c r="AZ33" s="73">
+        <v>30</v>
+      </c>
+      <c r="BA33" s="73">
+        <v>31</v>
+      </c>
+      <c r="BB33" s="90">
+        <v>32</v>
+      </c>
+      <c r="BC33" s="80">
+        <v>33</v>
+      </c>
+      <c r="BD33" s="73">
+        <v>34</v>
+      </c>
+      <c r="BE33" s="73">
+        <v>35</v>
+      </c>
+      <c r="BI33" s="94">
+        <v>29</v>
+      </c>
+      <c r="BJ33" s="88">
+        <v>30</v>
+      </c>
+      <c r="BK33" s="73">
+        <v>31</v>
+      </c>
+      <c r="BL33" s="73">
+        <v>32</v>
+      </c>
+      <c r="BM33" s="90">
+        <v>33</v>
+      </c>
+      <c r="BN33" s="80">
+        <v>34</v>
+      </c>
+      <c r="BO33" s="73">
+        <v>35</v>
+      </c>
+      <c r="BS33" s="73">
+        <v>29</v>
+      </c>
+      <c r="BT33" s="94">
+        <v>30</v>
+      </c>
+      <c r="BU33" s="88">
+        <v>31</v>
+      </c>
+      <c r="BV33" s="73">
+        <v>32</v>
+      </c>
+      <c r="BW33" s="73">
+        <v>33</v>
+      </c>
+      <c r="BX33" s="90">
+        <v>34</v>
+      </c>
+      <c r="BY33" s="80">
+        <v>35</v>
+      </c>
+      <c r="CC33" s="73">
+        <v>29</v>
+      </c>
+      <c r="CD33" s="73">
+        <v>30</v>
+      </c>
+      <c r="CE33" s="94">
+        <v>31</v>
+      </c>
+      <c r="CF33" s="88">
+        <v>32</v>
+      </c>
+      <c r="CG33" s="73">
+        <v>33</v>
+      </c>
+      <c r="CH33" s="73">
+        <v>34</v>
+      </c>
+      <c r="CI33" s="90">
+        <v>35</v>
+      </c>
+      <c r="CJ33" s="65"/>
+    </row>
+    <row r="34" spans="2:88" ht="16.3" customHeight="1" x14ac:dyDescent="0.45">
       <c r="B34" s="64"/>
       <c r="C34" s="88">
         <v>22</v>
@@ -7047,8 +9759,94 @@
         <v>28</v>
       </c>
       <c r="AT34" s="65"/>
-    </row>
-    <row r="35" spans="2:46" ht="16.3" customHeight="1" thickBot="1" x14ac:dyDescent="0.5">
+      <c r="AX34" s="64"/>
+      <c r="AY34" s="88">
+        <v>22</v>
+      </c>
+      <c r="AZ34" s="77">
+        <v>23</v>
+      </c>
+      <c r="BA34" s="77">
+        <v>24</v>
+      </c>
+      <c r="BB34" s="89">
+        <v>25</v>
+      </c>
+      <c r="BC34" s="81">
+        <v>26</v>
+      </c>
+      <c r="BD34" s="77">
+        <v>27</v>
+      </c>
+      <c r="BE34" s="74">
+        <v>28</v>
+      </c>
+      <c r="BI34" s="94">
+        <v>22</v>
+      </c>
+      <c r="BJ34" s="96">
+        <v>23</v>
+      </c>
+      <c r="BK34" s="77">
+        <v>24</v>
+      </c>
+      <c r="BL34" s="77">
+        <v>25</v>
+      </c>
+      <c r="BM34" s="89">
+        <v>26</v>
+      </c>
+      <c r="BN34" s="81">
+        <v>27</v>
+      </c>
+      <c r="BO34" s="74">
+        <v>28</v>
+      </c>
+      <c r="BS34" s="73">
+        <v>22</v>
+      </c>
+      <c r="BT34" s="97">
+        <v>23</v>
+      </c>
+      <c r="BU34" s="96">
+        <v>24</v>
+      </c>
+      <c r="BV34" s="77">
+        <v>25</v>
+      </c>
+      <c r="BW34" s="77">
+        <v>26</v>
+      </c>
+      <c r="BX34" s="89">
+        <v>27</v>
+      </c>
+      <c r="BY34" s="95">
+        <v>28</v>
+      </c>
+      <c r="CC34" s="73">
+        <v>22</v>
+      </c>
+      <c r="CD34" s="77">
+        <v>23</v>
+      </c>
+      <c r="CE34" s="97">
+        <v>24</v>
+      </c>
+      <c r="CF34" s="96">
+        <v>25</v>
+      </c>
+      <c r="CG34" s="77">
+        <v>26</v>
+      </c>
+      <c r="CH34" s="77">
+        <v>27</v>
+      </c>
+      <c r="CI34" s="99">
+        <v>28</v>
+      </c>
+      <c r="CJ34" s="65"/>
+    </row>
+    <row r="35" spans="2:88" ht="16.3" customHeight="1" thickBot="1" x14ac:dyDescent="0.5">
       <c r="B35" s="64"/>
       <c r="C35" s="91">
         <v>15</v>
@@ -7159,8 +9957,94 @@
         <v>21</v>
       </c>
       <c r="AT35" s="65"/>
-    </row>
-    <row r="36" spans="2:46" ht="16.3" customHeight="1" thickTop="1" x14ac:dyDescent="0.45">
+      <c r="AX35" s="64"/>
+      <c r="AY35" s="91">
+        <v>15</v>
+      </c>
+      <c r="AZ35" s="92">
+        <v>16</v>
+      </c>
+      <c r="BA35" s="92">
+        <v>17</v>
+      </c>
+      <c r="BB35" s="93">
+        <v>18</v>
+      </c>
+      <c r="BC35" s="80">
+        <v>19</v>
+      </c>
+      <c r="BD35" s="73">
+        <v>20</v>
+      </c>
+      <c r="BE35" s="73">
+        <v>21</v>
+      </c>
+      <c r="BI35" s="94">
+        <v>15</v>
+      </c>
+      <c r="BJ35" s="91">
+        <v>16</v>
+      </c>
+      <c r="BK35" s="92">
+        <v>17</v>
+      </c>
+      <c r="BL35" s="92">
+        <v>18</v>
+      </c>
+      <c r="BM35" s="93">
+        <v>19</v>
+      </c>
+      <c r="BN35" s="80">
+        <v>20</v>
+      </c>
+      <c r="BO35" s="73">
+        <v>21</v>
+      </c>
+      <c r="BS35" s="73">
+        <v>15</v>
+      </c>
+      <c r="BT35" s="94">
+        <v>16</v>
+      </c>
+      <c r="BU35" s="91">
+        <v>17</v>
+      </c>
+      <c r="BV35" s="92">
+        <v>18</v>
+      </c>
+      <c r="BW35" s="92">
+        <v>19</v>
+      </c>
+      <c r="BX35" s="93">
+        <v>20</v>
+      </c>
+      <c r="BY35" s="80">
+        <v>21</v>
+      </c>
+      <c r="CC35" s="73">
+        <v>15</v>
+      </c>
+      <c r="CD35" s="73">
+        <v>16</v>
+      </c>
+      <c r="CE35" s="94">
+        <v>17</v>
+      </c>
+      <c r="CF35" s="91">
+        <v>18</v>
+      </c>
+      <c r="CG35" s="92">
+        <v>19</v>
+      </c>
+      <c r="CH35" s="92">
+        <v>20</v>
+      </c>
+      <c r="CI35" s="93">
+        <v>21</v>
+      </c>
+      <c r="CJ35" s="65"/>
+    </row>
+    <row r="36" spans="2:88" ht="16.3" customHeight="1" thickTop="1" x14ac:dyDescent="0.45">
       <c r="C36" s="100">
         <v>8</v>
       </c>
@@ -7269,8 +10153,92 @@
       <c r="AS36" s="110">
         <v>14</v>
       </c>
-    </row>
-    <row r="37" spans="2:46" ht="16.3" customHeight="1" x14ac:dyDescent="0.45">
+      <c r="AY36" s="100">
+        <v>8</v>
+      </c>
+      <c r="AZ36" s="109">
+        <v>9</v>
+      </c>
+      <c r="BA36" s="109">
+        <v>10</v>
+      </c>
+      <c r="BB36" s="109">
+        <v>11</v>
+      </c>
+      <c r="BC36" s="77">
+        <v>12</v>
+      </c>
+      <c r="BD36" s="77">
+        <v>13</v>
+      </c>
+      <c r="BE36" s="74">
+        <v>14</v>
+      </c>
+      <c r="BI36" s="73">
+        <v>8</v>
+      </c>
+      <c r="BJ36" s="109">
+        <v>9</v>
+      </c>
+      <c r="BK36" s="109">
+        <v>10</v>
+      </c>
+      <c r="BL36" s="109">
+        <v>11</v>
+      </c>
+      <c r="BM36" s="109">
+        <v>12</v>
+      </c>
+      <c r="BN36" s="77">
+        <v>13</v>
+      </c>
+      <c r="BO36" s="74">
+        <v>14</v>
+      </c>
+      <c r="BS36" s="73">
+        <v>8</v>
+      </c>
+      <c r="BT36" s="77">
+        <v>9</v>
+      </c>
+      <c r="BU36" s="109">
+        <v>10</v>
+      </c>
+      <c r="BV36" s="109">
+        <v>11</v>
+      </c>
+      <c r="BW36" s="109">
+        <v>12</v>
+      </c>
+      <c r="BX36" s="109">
+        <v>13</v>
+      </c>
+      <c r="BY36" s="74">
+        <v>14</v>
+      </c>
+      <c r="CC36" s="73">
+        <v>8</v>
+      </c>
+      <c r="CD36" s="77">
+        <v>9</v>
+      </c>
+      <c r="CE36" s="77">
+        <v>10</v>
+      </c>
+      <c r="CF36" s="109">
+        <v>11</v>
+      </c>
+      <c r="CG36" s="109">
+        <v>12</v>
+      </c>
+      <c r="CH36" s="109">
+        <v>13</v>
+      </c>
+      <c r="CI36" s="110">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="37" spans="2:88" ht="16.3" customHeight="1" x14ac:dyDescent="0.45">
       <c r="C37" s="73">
         <v>1</v>
       </c>
@@ -7379,13 +10347,97 @@
       <c r="AS37" s="73">
         <v>7</v>
       </c>
-    </row>
-    <row r="38" spans="2:46" ht="16.3" customHeight="1" x14ac:dyDescent="0.45">
+      <c r="AY37" s="73">
+        <v>1</v>
+      </c>
+      <c r="AZ37" s="73">
+        <v>2</v>
+      </c>
+      <c r="BA37" s="73">
+        <v>3</v>
+      </c>
+      <c r="BB37" s="73">
+        <v>4</v>
+      </c>
+      <c r="BC37" s="73">
+        <v>5</v>
+      </c>
+      <c r="BD37" s="73">
+        <v>6</v>
+      </c>
+      <c r="BE37" s="73">
+        <v>7</v>
+      </c>
+      <c r="BI37" s="73">
+        <v>1</v>
+      </c>
+      <c r="BJ37" s="73">
+        <v>2</v>
+      </c>
+      <c r="BK37" s="73">
+        <v>3</v>
+      </c>
+      <c r="BL37" s="73">
+        <v>4</v>
+      </c>
+      <c r="BM37" s="73">
+        <v>5</v>
+      </c>
+      <c r="BN37" s="73">
+        <v>6</v>
+      </c>
+      <c r="BO37" s="73">
+        <v>7</v>
+      </c>
+      <c r="BS37" s="73">
+        <v>1</v>
+      </c>
+      <c r="BT37" s="73">
+        <v>2</v>
+      </c>
+      <c r="BU37" s="73">
+        <v>3</v>
+      </c>
+      <c r="BV37" s="73">
+        <v>4</v>
+      </c>
+      <c r="BW37" s="73">
+        <v>5</v>
+      </c>
+      <c r="BX37" s="73">
+        <v>6</v>
+      </c>
+      <c r="BY37" s="73">
+        <v>7</v>
+      </c>
+      <c r="CC37" s="73">
+        <v>1</v>
+      </c>
+      <c r="CD37" s="73">
+        <v>2</v>
+      </c>
+      <c r="CE37" s="73">
+        <v>3</v>
+      </c>
+      <c r="CF37" s="73">
+        <v>4</v>
+      </c>
+      <c r="CG37" s="73">
+        <v>5</v>
+      </c>
+      <c r="CH37" s="73">
+        <v>6</v>
+      </c>
+      <c r="CI37" s="73">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="38" spans="2:88" ht="16.3" customHeight="1" x14ac:dyDescent="0.45">
       <c r="C38" s="71"/>
       <c r="I38" s="71"/>
       <c r="O38" s="71"/>
     </row>
-    <row r="39" spans="2:46" x14ac:dyDescent="0.45">
+    <row r="39" spans="2:88" ht="15.6" thickBot="1" x14ac:dyDescent="0.5">
       <c r="C39" s="78" t="s">
         <v>15</v>
       </c>
@@ -7414,8 +10466,35 @@
       <c r="AM39" s="79" t="s">
         <v>19</v>
       </c>
-    </row>
-    <row r="40" spans="2:46" ht="15.6" thickBot="1" x14ac:dyDescent="0.5">
+      <c r="AY39" s="111" t="s">
+        <v>37</v>
+      </c>
+      <c r="AZ39" s="63"/>
+      <c r="BA39" s="63"/>
+      <c r="BB39" s="63"/>
+      <c r="BI39" s="79" t="s">
+        <v>38</v>
+      </c>
+      <c r="BJ39" s="63"/>
+      <c r="BK39" s="63"/>
+      <c r="BL39" s="63"/>
+      <c r="BM39" s="63"/>
+      <c r="BS39" s="79" t="s">
+        <v>39</v>
+      </c>
+      <c r="BU39" s="63"/>
+      <c r="BV39" s="63"/>
+      <c r="BW39" s="63"/>
+      <c r="BX39" s="63"/>
+      <c r="CC39" s="79" t="s">
+        <v>40</v>
+      </c>
+      <c r="CF39" s="63"/>
+      <c r="CG39" s="63"/>
+      <c r="CH39" s="63"/>
+      <c r="CI39" s="63"/>
+    </row>
+    <row r="40" spans="2:88" ht="15.9" thickTop="1" thickBot="1" x14ac:dyDescent="0.5">
       <c r="C40" s="82">
         <v>43</v>
       </c>
@@ -7524,8 +10603,94 @@
       <c r="AS40" s="82">
         <v>49</v>
       </c>
-    </row>
-    <row r="41" spans="2:46" ht="15.6" thickTop="1" x14ac:dyDescent="0.45">
+      <c r="AX40" s="64"/>
+      <c r="AY40" s="85">
+        <v>43</v>
+      </c>
+      <c r="AZ40" s="86">
+        <v>44</v>
+      </c>
+      <c r="BA40" s="86">
+        <v>45</v>
+      </c>
+      <c r="BB40" s="87">
+        <v>46</v>
+      </c>
+      <c r="BC40" s="80">
+        <v>47</v>
+      </c>
+      <c r="BD40" s="73">
+        <v>48</v>
+      </c>
+      <c r="BE40" s="73">
+        <v>49</v>
+      </c>
+      <c r="BI40" s="94">
+        <v>43</v>
+      </c>
+      <c r="BJ40" s="85">
+        <v>44</v>
+      </c>
+      <c r="BK40" s="86">
+        <v>45</v>
+      </c>
+      <c r="BL40" s="86">
+        <v>46</v>
+      </c>
+      <c r="BM40" s="87">
+        <v>47</v>
+      </c>
+      <c r="BN40" s="80">
+        <v>48</v>
+      </c>
+      <c r="BO40" s="73">
+        <v>49</v>
+      </c>
+      <c r="BS40" s="73">
+        <v>43</v>
+      </c>
+      <c r="BT40" s="94">
+        <v>44</v>
+      </c>
+      <c r="BU40" s="85">
+        <v>45</v>
+      </c>
+      <c r="BV40" s="86">
+        <v>46</v>
+      </c>
+      <c r="BW40" s="86">
+        <v>47</v>
+      </c>
+      <c r="BX40" s="87">
+        <v>48</v>
+      </c>
+      <c r="BY40" s="80">
+        <v>49</v>
+      </c>
+      <c r="CC40" s="73">
+        <v>43</v>
+      </c>
+      <c r="CD40" s="73">
+        <v>44</v>
+      </c>
+      <c r="CE40" s="94">
+        <v>45</v>
+      </c>
+      <c r="CF40" s="85">
+        <v>46</v>
+      </c>
+      <c r="CG40" s="86">
+        <v>47</v>
+      </c>
+      <c r="CH40" s="86">
+        <v>48</v>
+      </c>
+      <c r="CI40" s="87">
+        <v>49</v>
+      </c>
+      <c r="CJ40" s="65"/>
+    </row>
+    <row r="41" spans="2:88" ht="15.6" thickTop="1" x14ac:dyDescent="0.45">
       <c r="B41" s="64"/>
       <c r="C41" s="85">
         <v>36</v>
@@ -7636,8 +10801,94 @@
         <v>42</v>
       </c>
       <c r="AT41" s="65"/>
-    </row>
-    <row r="42" spans="2:46" x14ac:dyDescent="0.45">
+      <c r="AX41" s="64"/>
+      <c r="AY41" s="88">
+        <v>36</v>
+      </c>
+      <c r="AZ41" s="77">
+        <v>37</v>
+      </c>
+      <c r="BA41" s="77">
+        <v>38</v>
+      </c>
+      <c r="BB41" s="89">
+        <v>39</v>
+      </c>
+      <c r="BC41" s="81">
+        <v>40</v>
+      </c>
+      <c r="BD41" s="77">
+        <v>41</v>
+      </c>
+      <c r="BE41" s="74">
+        <v>42</v>
+      </c>
+      <c r="BI41" s="94">
+        <v>36</v>
+      </c>
+      <c r="BJ41" s="96">
+        <v>37</v>
+      </c>
+      <c r="BK41" s="77">
+        <v>38</v>
+      </c>
+      <c r="BL41" s="77">
+        <v>39</v>
+      </c>
+      <c r="BM41" s="89">
+        <v>40</v>
+      </c>
+      <c r="BN41" s="81">
+        <v>41</v>
+      </c>
+      <c r="BO41" s="74">
+        <v>42</v>
+      </c>
+      <c r="BS41" s="73">
+        <v>36</v>
+      </c>
+      <c r="BT41" s="97">
+        <v>37</v>
+      </c>
+      <c r="BU41" s="96">
+        <v>38</v>
+      </c>
+      <c r="BV41" s="77">
+        <v>39</v>
+      </c>
+      <c r="BW41" s="77">
+        <v>40</v>
+      </c>
+      <c r="BX41" s="89">
+        <v>41</v>
+      </c>
+      <c r="BY41" s="95">
+        <v>42</v>
+      </c>
+      <c r="CC41" s="73">
+        <v>36</v>
+      </c>
+      <c r="CD41" s="77">
+        <v>37</v>
+      </c>
+      <c r="CE41" s="97">
+        <v>38</v>
+      </c>
+      <c r="CF41" s="96">
+        <v>39</v>
+      </c>
+      <c r="CG41" s="77">
+        <v>40</v>
+      </c>
+      <c r="CH41" s="77">
+        <v>41</v>
+      </c>
+      <c r="CI41" s="99">
+        <v>42</v>
+      </c>
+      <c r="CJ41" s="65"/>
+    </row>
+    <row r="42" spans="2:88" x14ac:dyDescent="0.45">
       <c r="B42" s="64"/>
       <c r="C42" s="88">
         <v>29</v>
@@ -7748,8 +10999,94 @@
         <v>35</v>
       </c>
       <c r="AT42" s="65"/>
-    </row>
-    <row r="43" spans="2:46" ht="15.6" thickBot="1" x14ac:dyDescent="0.5">
+      <c r="AX42" s="64"/>
+      <c r="AY42" s="88">
+        <v>29</v>
+      </c>
+      <c r="AZ42" s="73">
+        <v>30</v>
+      </c>
+      <c r="BA42" s="73">
+        <v>31</v>
+      </c>
+      <c r="BB42" s="90">
+        <v>32</v>
+      </c>
+      <c r="BC42" s="80">
+        <v>33</v>
+      </c>
+      <c r="BD42" s="73">
+        <v>34</v>
+      </c>
+      <c r="BE42" s="73">
+        <v>35</v>
+      </c>
+      <c r="BI42" s="94">
+        <v>29</v>
+      </c>
+      <c r="BJ42" s="88">
+        <v>30</v>
+      </c>
+      <c r="BK42" s="73">
+        <v>31</v>
+      </c>
+      <c r="BL42" s="73">
+        <v>32</v>
+      </c>
+      <c r="BM42" s="90">
+        <v>33</v>
+      </c>
+      <c r="BN42" s="80">
+        <v>34</v>
+      </c>
+      <c r="BO42" s="73">
+        <v>35</v>
+      </c>
+      <c r="BS42" s="73">
+        <v>29</v>
+      </c>
+      <c r="BT42" s="94">
+        <v>30</v>
+      </c>
+      <c r="BU42" s="88">
+        <v>31</v>
+      </c>
+      <c r="BV42" s="73">
+        <v>32</v>
+      </c>
+      <c r="BW42" s="73">
+        <v>33</v>
+      </c>
+      <c r="BX42" s="90">
+        <v>34</v>
+      </c>
+      <c r="BY42" s="80">
+        <v>35</v>
+      </c>
+      <c r="CC42" s="73">
+        <v>29</v>
+      </c>
+      <c r="CD42" s="73">
+        <v>30</v>
+      </c>
+      <c r="CE42" s="94">
+        <v>31</v>
+      </c>
+      <c r="CF42" s="88">
+        <v>32</v>
+      </c>
+      <c r="CG42" s="73">
+        <v>33</v>
+      </c>
+      <c r="CH42" s="73">
+        <v>34</v>
+      </c>
+      <c r="CI42" s="90">
+        <v>35</v>
+      </c>
+      <c r="CJ42" s="65"/>
+    </row>
+    <row r="43" spans="2:88" ht="15.6" thickBot="1" x14ac:dyDescent="0.5">
       <c r="B43" s="64"/>
       <c r="C43" s="91">
         <v>22</v>
@@ -7860,8 +11197,94 @@
         <v>28</v>
       </c>
       <c r="AT43" s="65"/>
-    </row>
-    <row r="44" spans="2:46" ht="15.6" thickTop="1" x14ac:dyDescent="0.45">
+      <c r="AX43" s="64"/>
+      <c r="AY43" s="91">
+        <v>22</v>
+      </c>
+      <c r="AZ43" s="103">
+        <v>23</v>
+      </c>
+      <c r="BA43" s="103">
+        <v>24</v>
+      </c>
+      <c r="BB43" s="104">
+        <v>25</v>
+      </c>
+      <c r="BC43" s="81">
+        <v>26</v>
+      </c>
+      <c r="BD43" s="77">
+        <v>27</v>
+      </c>
+      <c r="BE43" s="74">
+        <v>28</v>
+      </c>
+      <c r="BI43" s="94">
+        <v>22</v>
+      </c>
+      <c r="BJ43" s="106">
+        <v>23</v>
+      </c>
+      <c r="BK43" s="103">
+        <v>24</v>
+      </c>
+      <c r="BL43" s="103">
+        <v>25</v>
+      </c>
+      <c r="BM43" s="104">
+        <v>26</v>
+      </c>
+      <c r="BN43" s="81">
+        <v>27</v>
+      </c>
+      <c r="BO43" s="74">
+        <v>28</v>
+      </c>
+      <c r="BS43" s="73">
+        <v>22</v>
+      </c>
+      <c r="BT43" s="97">
+        <v>23</v>
+      </c>
+      <c r="BU43" s="106">
+        <v>24</v>
+      </c>
+      <c r="BV43" s="103">
+        <v>25</v>
+      </c>
+      <c r="BW43" s="103">
+        <v>26</v>
+      </c>
+      <c r="BX43" s="104">
+        <v>27</v>
+      </c>
+      <c r="BY43" s="95">
+        <v>28</v>
+      </c>
+      <c r="CC43" s="73">
+        <v>22</v>
+      </c>
+      <c r="CD43" s="77">
+        <v>23</v>
+      </c>
+      <c r="CE43" s="97">
+        <v>24</v>
+      </c>
+      <c r="CF43" s="106">
+        <v>25</v>
+      </c>
+      <c r="CG43" s="103">
+        <v>26</v>
+      </c>
+      <c r="CH43" s="103">
+        <v>27</v>
+      </c>
+      <c r="CI43" s="108">
+        <v>28</v>
+      </c>
+      <c r="CJ43" s="65"/>
+    </row>
+    <row r="44" spans="2:88" ht="15.6" thickTop="1" x14ac:dyDescent="0.45">
       <c r="C44" s="100">
         <v>15</v>
       </c>
@@ -7967,8 +11390,92 @@
       <c r="AS44" s="100">
         <v>21</v>
       </c>
-    </row>
-    <row r="45" spans="2:46" x14ac:dyDescent="0.45">
+      <c r="AY44" s="100">
+        <v>15</v>
+      </c>
+      <c r="AZ44" s="100">
+        <v>16</v>
+      </c>
+      <c r="BA44" s="100">
+        <v>17</v>
+      </c>
+      <c r="BB44" s="100">
+        <v>18</v>
+      </c>
+      <c r="BC44" s="73">
+        <v>19</v>
+      </c>
+      <c r="BD44" s="73">
+        <v>20</v>
+      </c>
+      <c r="BE44" s="73">
+        <v>21</v>
+      </c>
+      <c r="BI44" s="73">
+        <v>15</v>
+      </c>
+      <c r="BJ44" s="100">
+        <v>16</v>
+      </c>
+      <c r="BK44" s="100">
+        <v>17</v>
+      </c>
+      <c r="BL44" s="100">
+        <v>18</v>
+      </c>
+      <c r="BM44" s="100">
+        <v>19</v>
+      </c>
+      <c r="BN44" s="73">
+        <v>20</v>
+      </c>
+      <c r="BO44" s="73">
+        <v>21</v>
+      </c>
+      <c r="BS44" s="73">
+        <v>15</v>
+      </c>
+      <c r="BT44" s="73">
+        <v>16</v>
+      </c>
+      <c r="BU44" s="100">
+        <v>17</v>
+      </c>
+      <c r="BV44" s="100">
+        <v>18</v>
+      </c>
+      <c r="BW44" s="100">
+        <v>19</v>
+      </c>
+      <c r="BX44" s="100">
+        <v>20</v>
+      </c>
+      <c r="BY44" s="73">
+        <v>21</v>
+      </c>
+      <c r="CC44" s="73">
+        <v>15</v>
+      </c>
+      <c r="CD44" s="73">
+        <v>16</v>
+      </c>
+      <c r="CE44" s="73">
+        <v>17</v>
+      </c>
+      <c r="CF44" s="100">
+        <v>18</v>
+      </c>
+      <c r="CG44" s="100">
+        <v>19</v>
+      </c>
+      <c r="CH44" s="100">
+        <v>20</v>
+      </c>
+      <c r="CI44" s="100">
+        <v>21</v>
+      </c>
+    </row>
+    <row r="45" spans="2:88" x14ac:dyDescent="0.45">
       <c r="C45" s="73">
         <v>8</v>
       </c>
@@ -8074,8 +11581,92 @@
       <c r="AS45" s="74">
         <v>14</v>
       </c>
-    </row>
-    <row r="46" spans="2:46" x14ac:dyDescent="0.45">
+      <c r="AY45" s="73">
+        <v>8</v>
+      </c>
+      <c r="AZ45" s="77">
+        <v>9</v>
+      </c>
+      <c r="BA45" s="77">
+        <v>10</v>
+      </c>
+      <c r="BB45" s="77">
+        <v>11</v>
+      </c>
+      <c r="BC45" s="77">
+        <v>12</v>
+      </c>
+      <c r="BD45" s="77">
+        <v>13</v>
+      </c>
+      <c r="BE45" s="74">
+        <v>14</v>
+      </c>
+      <c r="BI45" s="73">
+        <v>8</v>
+      </c>
+      <c r="BJ45" s="77">
+        <v>9</v>
+      </c>
+      <c r="BK45" s="77">
+        <v>10</v>
+      </c>
+      <c r="BL45" s="77">
+        <v>11</v>
+      </c>
+      <c r="BM45" s="77">
+        <v>12</v>
+      </c>
+      <c r="BN45" s="77">
+        <v>13</v>
+      </c>
+      <c r="BO45" s="74">
+        <v>14</v>
+      </c>
+      <c r="BS45" s="73">
+        <v>8</v>
+      </c>
+      <c r="BT45" s="77">
+        <v>9</v>
+      </c>
+      <c r="BU45" s="77">
+        <v>10</v>
+      </c>
+      <c r="BV45" s="77">
+        <v>11</v>
+      </c>
+      <c r="BW45" s="77">
+        <v>12</v>
+      </c>
+      <c r="BX45" s="77">
+        <v>13</v>
+      </c>
+      <c r="BY45" s="74">
+        <v>14</v>
+      </c>
+      <c r="CC45" s="73">
+        <v>8</v>
+      </c>
+      <c r="CD45" s="77">
+        <v>9</v>
+      </c>
+      <c r="CE45" s="77">
+        <v>10</v>
+      </c>
+      <c r="CF45" s="77">
+        <v>11</v>
+      </c>
+      <c r="CG45" s="77">
+        <v>12</v>
+      </c>
+      <c r="CH45" s="77">
+        <v>13</v>
+      </c>
+      <c r="CI45" s="74">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="46" spans="2:88" x14ac:dyDescent="0.45">
       <c r="C46" s="73">
         <v>1</v>
       </c>
@@ -8186,8 +11777,92 @@
       <c r="AS46" s="73">
         <v>7</v>
       </c>
-    </row>
-    <row r="48" spans="2:46" ht="15.6" thickBot="1" x14ac:dyDescent="0.5">
+      <c r="AY46" s="73">
+        <v>1</v>
+      </c>
+      <c r="AZ46" s="73">
+        <v>2</v>
+      </c>
+      <c r="BA46" s="73">
+        <v>3</v>
+      </c>
+      <c r="BB46" s="73">
+        <v>4</v>
+      </c>
+      <c r="BC46" s="73">
+        <v>5</v>
+      </c>
+      <c r="BD46" s="73">
+        <v>6</v>
+      </c>
+      <c r="BE46" s="73">
+        <v>7</v>
+      </c>
+      <c r="BI46" s="73">
+        <v>1</v>
+      </c>
+      <c r="BJ46" s="73">
+        <v>2</v>
+      </c>
+      <c r="BK46" s="73">
+        <v>3</v>
+      </c>
+      <c r="BL46" s="73">
+        <v>4</v>
+      </c>
+      <c r="BM46" s="73">
+        <v>5</v>
+      </c>
+      <c r="BN46" s="73">
+        <v>6</v>
+      </c>
+      <c r="BO46" s="73">
+        <v>7</v>
+      </c>
+      <c r="BS46" s="73">
+        <v>1</v>
+      </c>
+      <c r="BT46" s="73">
+        <v>2</v>
+      </c>
+      <c r="BU46" s="73">
+        <v>3</v>
+      </c>
+      <c r="BV46" s="73">
+        <v>4</v>
+      </c>
+      <c r="BW46" s="73">
+        <v>5</v>
+      </c>
+      <c r="BX46" s="73">
+        <v>6</v>
+      </c>
+      <c r="BY46" s="73">
+        <v>7</v>
+      </c>
+      <c r="CC46" s="73">
+        <v>1</v>
+      </c>
+      <c r="CD46" s="73">
+        <v>2</v>
+      </c>
+      <c r="CE46" s="73">
+        <v>3</v>
+      </c>
+      <c r="CF46" s="73">
+        <v>4</v>
+      </c>
+      <c r="CG46" s="73">
+        <v>5</v>
+      </c>
+      <c r="CH46" s="73">
+        <v>6</v>
+      </c>
+      <c r="CI46" s="73">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="48" spans="2:88" ht="15.6" thickBot="1" x14ac:dyDescent="0.5">
       <c r="C48" s="111" t="s">
         <v>20</v>
       </c>

</xml_diff>